<commit_message>
Updated on 02-14-2024 at 23:52
</commit_message>
<xml_diff>
--- a/experiment_2/data/br.xlsx
+++ b/experiment_2/data/br.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\gustavo\github\LOVO\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\gustavo\github\LOVO2024\experiment_2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36616B-0164-4722-950E-90150E60C458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E1FBE7-5EBF-4C7D-BAC2-6B8343DE5D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4283,12 +4283,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4318,11 +4330,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4452,8 +4466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q1393"/>
+    <sheetView tabSelected="1" topLeftCell="A483" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91:D490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8179,7 +8193,7 @@
       <c r="C91" t="s">
         <v>1411</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E91">
@@ -8232,7 +8246,7 @@
       <c r="C92" t="s">
         <v>1411</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E92">
@@ -8285,7 +8299,7 @@
       <c r="C93" t="s">
         <v>1411</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E93">
@@ -8338,7 +8352,7 @@
       <c r="C94" t="s">
         <v>1411</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E94">
@@ -8391,7 +8405,7 @@
       <c r="C95" t="s">
         <v>1411</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E95">
@@ -8444,7 +8458,7 @@
       <c r="C96" t="s">
         <v>1411</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E96">
@@ -8497,7 +8511,7 @@
       <c r="C97" t="s">
         <v>1411</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E97">
@@ -8550,7 +8564,7 @@
       <c r="C98" t="s">
         <v>1411</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="2" t="s">
         <v>114</v>
       </c>
       <c r="E98">
@@ -8603,7 +8617,7 @@
       <c r="C99" t="s">
         <v>1411</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E99">
@@ -8656,7 +8670,7 @@
       <c r="C100" t="s">
         <v>1411</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E100">
@@ -8709,7 +8723,7 @@
       <c r="C101" t="s">
         <v>1411</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E101">
@@ -8762,7 +8776,7 @@
       <c r="C102" t="s">
         <v>1411</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E102">
@@ -8815,7 +8829,7 @@
       <c r="C103" t="s">
         <v>1411</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E103">
@@ -8868,7 +8882,7 @@
       <c r="C104" t="s">
         <v>1411</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E104">
@@ -8921,7 +8935,7 @@
       <c r="C105" t="s">
         <v>1411</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E105">
@@ -8974,7 +8988,7 @@
       <c r="C106" t="s">
         <v>1411</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E106">
@@ -9027,7 +9041,7 @@
       <c r="C107" t="s">
         <v>1411</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="2" t="s">
         <v>123</v>
       </c>
       <c r="E107">
@@ -9080,7 +9094,7 @@
       <c r="C108" t="s">
         <v>1411</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E108">
@@ -9133,7 +9147,7 @@
       <c r="C109" t="s">
         <v>1411</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E109">
@@ -9186,7 +9200,7 @@
       <c r="C110" t="s">
         <v>1411</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E110">
@@ -9239,7 +9253,7 @@
       <c r="C111" t="s">
         <v>1411</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="2" t="s">
         <v>127</v>
       </c>
       <c r="E111">
@@ -9292,7 +9306,7 @@
       <c r="C112" t="s">
         <v>1411</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E112">
@@ -9345,7 +9359,7 @@
       <c r="C113" t="s">
         <v>1411</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E113">
@@ -9398,7 +9412,7 @@
       <c r="C114" t="s">
         <v>1411</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E114">
@@ -9451,7 +9465,7 @@
       <c r="C115" t="s">
         <v>1411</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E115">
@@ -9504,7 +9518,7 @@
       <c r="C116" t="s">
         <v>1411</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E116">
@@ -9557,7 +9571,7 @@
       <c r="C117" t="s">
         <v>1411</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E117">
@@ -9610,7 +9624,7 @@
       <c r="C118" t="s">
         <v>1411</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E118">
@@ -9663,7 +9677,7 @@
       <c r="C119" t="s">
         <v>1411</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E119">
@@ -9716,7 +9730,7 @@
       <c r="C120" t="s">
         <v>1411</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E120">
@@ -9769,7 +9783,7 @@
       <c r="C121" t="s">
         <v>1411</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E121">
@@ -9822,7 +9836,7 @@
       <c r="C122" t="s">
         <v>1411</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="3" t="s">
         <v>138</v>
       </c>
       <c r="E122">
@@ -9875,7 +9889,7 @@
       <c r="C123" t="s">
         <v>1411</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="3" t="s">
         <v>139</v>
       </c>
       <c r="E123">
@@ -9928,7 +9942,7 @@
       <c r="C124" t="s">
         <v>1411</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="3" t="s">
         <v>140</v>
       </c>
       <c r="E124">
@@ -9981,7 +9995,7 @@
       <c r="C125" t="s">
         <v>1411</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E125">
@@ -10034,7 +10048,7 @@
       <c r="C126" t="s">
         <v>1411</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E126">
@@ -10087,7 +10101,7 @@
       <c r="C127" t="s">
         <v>1411</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E127">
@@ -10140,7 +10154,7 @@
       <c r="C128" t="s">
         <v>1411</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E128">
@@ -10193,7 +10207,7 @@
       <c r="C129" t="s">
         <v>1411</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E129">
@@ -10246,7 +10260,7 @@
       <c r="C130" t="s">
         <v>1411</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E130">
@@ -10299,7 +10313,7 @@
       <c r="C131" t="s">
         <v>1411</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E131">
@@ -10352,7 +10366,7 @@
       <c r="C132" t="s">
         <v>1411</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E132">
@@ -10405,7 +10419,7 @@
       <c r="C133" t="s">
         <v>1411</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E133">
@@ -10458,7 +10472,7 @@
       <c r="C134" t="s">
         <v>1411</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="2" t="s">
         <v>150</v>
       </c>
       <c r="E134">
@@ -10511,7 +10525,7 @@
       <c r="C135" t="s">
         <v>1411</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="2" t="s">
         <v>151</v>
       </c>
       <c r="E135">
@@ -10564,7 +10578,7 @@
       <c r="C136" t="s">
         <v>1411</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E136">
@@ -10617,7 +10631,7 @@
       <c r="C137" t="s">
         <v>1411</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="2" t="s">
         <v>153</v>
       </c>
       <c r="E137">
@@ -10670,7 +10684,7 @@
       <c r="C138" t="s">
         <v>1411</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E138">
@@ -10723,7 +10737,7 @@
       <c r="C139" t="s">
         <v>1411</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E139">
@@ -10776,7 +10790,7 @@
       <c r="C140" t="s">
         <v>1411</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="2" t="s">
         <v>156</v>
       </c>
       <c r="E140">
@@ -10829,7 +10843,7 @@
       <c r="C141" t="s">
         <v>1411</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E141">
@@ -10882,7 +10896,7 @@
       <c r="C142" t="s">
         <v>1411</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="2" t="s">
         <v>158</v>
       </c>
       <c r="E142">
@@ -10935,7 +10949,7 @@
       <c r="C143" t="s">
         <v>1411</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E143">
@@ -10988,7 +11002,7 @@
       <c r="C144" t="s">
         <v>1411</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E144">
@@ -11041,7 +11055,7 @@
       <c r="C145" t="s">
         <v>1411</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="2" t="s">
         <v>161</v>
       </c>
       <c r="E145">
@@ -11094,7 +11108,7 @@
       <c r="C146" t="s">
         <v>1411</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="2" t="s">
         <v>162</v>
       </c>
       <c r="E146">
@@ -11147,7 +11161,7 @@
       <c r="C147" t="s">
         <v>1411</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="2" t="s">
         <v>163</v>
       </c>
       <c r="E147">
@@ -11200,7 +11214,7 @@
       <c r="C148" t="s">
         <v>1411</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="2" t="s">
         <v>164</v>
       </c>
       <c r="E148">
@@ -11253,7 +11267,7 @@
       <c r="C149" t="s">
         <v>1411</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="2" t="s">
         <v>165</v>
       </c>
       <c r="E149">
@@ -11306,7 +11320,7 @@
       <c r="C150" t="s">
         <v>1411</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="2" t="s">
         <v>166</v>
       </c>
       <c r="E150">
@@ -11359,7 +11373,7 @@
       <c r="C151" t="s">
         <v>1411</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="2" t="s">
         <v>167</v>
       </c>
       <c r="E151">
@@ -11412,7 +11426,7 @@
       <c r="C152" t="s">
         <v>1411</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="2" t="s">
         <v>168</v>
       </c>
       <c r="E152">
@@ -11465,7 +11479,7 @@
       <c r="C153" t="s">
         <v>1411</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="2" t="s">
         <v>169</v>
       </c>
       <c r="E153">
@@ -11518,7 +11532,7 @@
       <c r="C154" t="s">
         <v>1411</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="2" t="s">
         <v>170</v>
       </c>
       <c r="E154">
@@ -11571,7 +11585,7 @@
       <c r="C155" t="s">
         <v>1411</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="2" t="s">
         <v>171</v>
       </c>
       <c r="E155">
@@ -11624,7 +11638,7 @@
       <c r="C156" t="s">
         <v>1411</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="2" t="s">
         <v>172</v>
       </c>
       <c r="E156">
@@ -11677,7 +11691,7 @@
       <c r="C157" t="s">
         <v>1411</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="2" t="s">
         <v>173</v>
       </c>
       <c r="E157">
@@ -11730,7 +11744,7 @@
       <c r="C158" t="s">
         <v>1411</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="2" t="s">
         <v>174</v>
       </c>
       <c r="E158">
@@ -11783,7 +11797,7 @@
       <c r="C159" t="s">
         <v>1411</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E159">
@@ -11836,7 +11850,7 @@
       <c r="C160" t="s">
         <v>1411</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="2" t="s">
         <v>176</v>
       </c>
       <c r="E160">
@@ -11889,7 +11903,7 @@
       <c r="C161" t="s">
         <v>1411</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E161">
@@ -11942,7 +11956,7 @@
       <c r="C162" t="s">
         <v>1411</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="3" t="s">
         <v>178</v>
       </c>
       <c r="E162">
@@ -11995,7 +12009,7 @@
       <c r="C163" t="s">
         <v>1411</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E163">
@@ -12048,7 +12062,7 @@
       <c r="C164" t="s">
         <v>1411</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="3" t="s">
         <v>180</v>
       </c>
       <c r="E164">
@@ -12101,7 +12115,7 @@
       <c r="C165" t="s">
         <v>1411</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="3" t="s">
         <v>181</v>
       </c>
       <c r="E165">
@@ -12154,7 +12168,7 @@
       <c r="C166" t="s">
         <v>1411</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="3" t="s">
         <v>182</v>
       </c>
       <c r="E166">
@@ -12207,7 +12221,7 @@
       <c r="C167" t="s">
         <v>1411</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="3" t="s">
         <v>183</v>
       </c>
       <c r="E167">
@@ -12260,7 +12274,7 @@
       <c r="C168" t="s">
         <v>1411</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E168">
@@ -12313,7 +12327,7 @@
       <c r="C169" t="s">
         <v>1411</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="3" t="s">
         <v>185</v>
       </c>
       <c r="E169">
@@ -12366,7 +12380,7 @@
       <c r="C170" t="s">
         <v>1411</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E170">
@@ -12419,7 +12433,7 @@
       <c r="C171" t="s">
         <v>1411</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E171">
@@ -12472,7 +12486,7 @@
       <c r="C172" t="s">
         <v>1411</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E172">
@@ -12525,7 +12539,7 @@
       <c r="C173" t="s">
         <v>1411</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="2" t="s">
         <v>189</v>
       </c>
       <c r="E173">
@@ -12578,7 +12592,7 @@
       <c r="C174" t="s">
         <v>1411</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="2" t="s">
         <v>190</v>
       </c>
       <c r="E174">
@@ -12631,7 +12645,7 @@
       <c r="C175" t="s">
         <v>1411</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="2" t="s">
         <v>191</v>
       </c>
       <c r="E175">
@@ -12684,7 +12698,7 @@
       <c r="C176" t="s">
         <v>1411</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="2" t="s">
         <v>192</v>
       </c>
       <c r="E176">
@@ -12737,7 +12751,7 @@
       <c r="C177" t="s">
         <v>1411</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="2" t="s">
         <v>193</v>
       </c>
       <c r="E177">
@@ -12790,7 +12804,7 @@
       <c r="C178" t="s">
         <v>1411</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E178">
@@ -12843,7 +12857,7 @@
       <c r="C179" t="s">
         <v>1411</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="2" t="s">
         <v>195</v>
       </c>
       <c r="E179">
@@ -12896,7 +12910,7 @@
       <c r="C180" t="s">
         <v>1411</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E180">
@@ -12949,7 +12963,7 @@
       <c r="C181" t="s">
         <v>1411</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="2" t="s">
         <v>197</v>
       </c>
       <c r="E181">
@@ -13002,7 +13016,7 @@
       <c r="C182" t="s">
         <v>1411</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="2" t="s">
         <v>198</v>
       </c>
       <c r="E182">
@@ -13055,7 +13069,7 @@
       <c r="C183" t="s">
         <v>1411</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="2" t="s">
         <v>199</v>
       </c>
       <c r="E183">
@@ -13108,7 +13122,7 @@
       <c r="C184" t="s">
         <v>1411</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="2" t="s">
         <v>200</v>
       </c>
       <c r="E184">
@@ -13161,7 +13175,7 @@
       <c r="C185" t="s">
         <v>1411</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="2" t="s">
         <v>201</v>
       </c>
       <c r="E185">
@@ -13214,7 +13228,7 @@
       <c r="C186" t="s">
         <v>1411</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="2" t="s">
         <v>202</v>
       </c>
       <c r="E186">
@@ -13267,7 +13281,7 @@
       <c r="C187" t="s">
         <v>1411</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="2" t="s">
         <v>203</v>
       </c>
       <c r="E187">
@@ -13320,7 +13334,7 @@
       <c r="C188" t="s">
         <v>1411</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="2" t="s">
         <v>204</v>
       </c>
       <c r="E188">
@@ -13373,7 +13387,7 @@
       <c r="C189" t="s">
         <v>1411</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="2" t="s">
         <v>205</v>
       </c>
       <c r="E189">
@@ -13426,7 +13440,7 @@
       <c r="C190" t="s">
         <v>1411</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="2" t="s">
         <v>206</v>
       </c>
       <c r="E190">
@@ -13479,7 +13493,7 @@
       <c r="C191" t="s">
         <v>1411</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="2" t="s">
         <v>207</v>
       </c>
       <c r="E191">
@@ -13532,7 +13546,7 @@
       <c r="C192" t="s">
         <v>1411</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="2" t="s">
         <v>208</v>
       </c>
       <c r="E192">
@@ -13585,7 +13599,7 @@
       <c r="C193" t="s">
         <v>1411</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="2" t="s">
         <v>209</v>
       </c>
       <c r="E193">
@@ -13638,7 +13652,7 @@
       <c r="C194" t="s">
         <v>1411</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E194">
@@ -13691,7 +13705,7 @@
       <c r="C195" t="s">
         <v>1411</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="2" t="s">
         <v>211</v>
       </c>
       <c r="E195">
@@ -13744,7 +13758,7 @@
       <c r="C196" t="s">
         <v>1411</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="2" t="s">
         <v>212</v>
       </c>
       <c r="E196">
@@ -13797,7 +13811,7 @@
       <c r="C197" t="s">
         <v>1411</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="2" t="s">
         <v>213</v>
       </c>
       <c r="E197">
@@ -13850,7 +13864,7 @@
       <c r="C198" t="s">
         <v>1411</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="2" t="s">
         <v>214</v>
       </c>
       <c r="E198">
@@ -13903,7 +13917,7 @@
       <c r="C199" t="s">
         <v>1411</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="2" t="s">
         <v>215</v>
       </c>
       <c r="E199">
@@ -13956,7 +13970,7 @@
       <c r="C200" t="s">
         <v>1411</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E200">
@@ -14009,7 +14023,7 @@
       <c r="C201" t="s">
         <v>1411</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="3" t="s">
         <v>217</v>
       </c>
       <c r="E201">
@@ -14062,7 +14076,7 @@
       <c r="C202" t="s">
         <v>1411</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="3" t="s">
         <v>218</v>
       </c>
       <c r="E202">
@@ -14115,7 +14129,7 @@
       <c r="C203" t="s">
         <v>1411</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="3" t="s">
         <v>219</v>
       </c>
       <c r="E203">
@@ -14168,7 +14182,7 @@
       <c r="C204" t="s">
         <v>1411</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="3" t="s">
         <v>220</v>
       </c>
       <c r="E204">
@@ -14221,7 +14235,7 @@
       <c r="C205" t="s">
         <v>1411</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="3" t="s">
         <v>221</v>
       </c>
       <c r="E205">
@@ -14274,7 +14288,7 @@
       <c r="C206" t="s">
         <v>1411</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="3" t="s">
         <v>222</v>
       </c>
       <c r="E206">
@@ -14327,7 +14341,7 @@
       <c r="C207" t="s">
         <v>1411</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="3" t="s">
         <v>223</v>
       </c>
       <c r="E207">
@@ -14380,7 +14394,7 @@
       <c r="C208" t="s">
         <v>1411</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="3" t="s">
         <v>224</v>
       </c>
       <c r="E208">
@@ -14433,7 +14447,7 @@
       <c r="C209" t="s">
         <v>1411</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="3" t="s">
         <v>225</v>
       </c>
       <c r="E209">
@@ -14486,7 +14500,7 @@
       <c r="C210" t="s">
         <v>1411</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="3" t="s">
         <v>226</v>
       </c>
       <c r="E210">
@@ -14539,7 +14553,7 @@
       <c r="C211" t="s">
         <v>1411</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="2" t="s">
         <v>227</v>
       </c>
       <c r="E211">
@@ -14592,7 +14606,7 @@
       <c r="C212" t="s">
         <v>1411</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="2" t="s">
         <v>228</v>
       </c>
       <c r="E212">
@@ -14645,7 +14659,7 @@
       <c r="C213" t="s">
         <v>1411</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="2" t="s">
         <v>229</v>
       </c>
       <c r="E213">
@@ -14698,7 +14712,7 @@
       <c r="C214" t="s">
         <v>1411</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="2" t="s">
         <v>230</v>
       </c>
       <c r="E214">
@@ -14751,7 +14765,7 @@
       <c r="C215" t="s">
         <v>1411</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="2" t="s">
         <v>231</v>
       </c>
       <c r="E215">
@@ -14804,7 +14818,7 @@
       <c r="C216" t="s">
         <v>1411</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="2" t="s">
         <v>232</v>
       </c>
       <c r="E216">
@@ -14857,7 +14871,7 @@
       <c r="C217" t="s">
         <v>1411</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="2" t="s">
         <v>233</v>
       </c>
       <c r="E217">
@@ -14910,7 +14924,7 @@
       <c r="C218" t="s">
         <v>1411</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="2" t="s">
         <v>234</v>
       </c>
       <c r="E218">
@@ -14963,7 +14977,7 @@
       <c r="C219" t="s">
         <v>1411</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="2" t="s">
         <v>235</v>
       </c>
       <c r="E219">
@@ -15016,7 +15030,7 @@
       <c r="C220" t="s">
         <v>1411</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="2" t="s">
         <v>236</v>
       </c>
       <c r="E220">
@@ -15069,7 +15083,7 @@
       <c r="C221" t="s">
         <v>1411</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="2" t="s">
         <v>237</v>
       </c>
       <c r="E221">
@@ -15122,7 +15136,7 @@
       <c r="C222" t="s">
         <v>1411</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="2" t="s">
         <v>238</v>
       </c>
       <c r="E222">
@@ -15175,7 +15189,7 @@
       <c r="C223" t="s">
         <v>1411</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="2" t="s">
         <v>239</v>
       </c>
       <c r="E223">
@@ -15228,7 +15242,7 @@
       <c r="C224" t="s">
         <v>1411</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="2" t="s">
         <v>240</v>
       </c>
       <c r="E224">
@@ -15281,7 +15295,7 @@
       <c r="C225" t="s">
         <v>1411</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E225">
@@ -15334,7 +15348,7 @@
       <c r="C226" t="s">
         <v>1411</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="2" t="s">
         <v>242</v>
       </c>
       <c r="E226">
@@ -15387,7 +15401,7 @@
       <c r="C227" t="s">
         <v>1411</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="2" t="s">
         <v>243</v>
       </c>
       <c r="E227">
@@ -15440,7 +15454,7 @@
       <c r="C228" t="s">
         <v>1411</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="2" t="s">
         <v>244</v>
       </c>
       <c r="E228">
@@ -15493,7 +15507,7 @@
       <c r="C229" t="s">
         <v>1411</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="2" t="s">
         <v>245</v>
       </c>
       <c r="E229">
@@ -15546,7 +15560,7 @@
       <c r="C230" t="s">
         <v>1411</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="2" t="s">
         <v>246</v>
       </c>
       <c r="E230">
@@ -15599,7 +15613,7 @@
       <c r="C231" t="s">
         <v>1411</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="2" t="s">
         <v>247</v>
       </c>
       <c r="E231">
@@ -15652,7 +15666,7 @@
       <c r="C232" t="s">
         <v>1411</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="2" t="s">
         <v>248</v>
       </c>
       <c r="E232">
@@ -15705,7 +15719,7 @@
       <c r="C233" t="s">
         <v>1411</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="2" t="s">
         <v>249</v>
       </c>
       <c r="E233">
@@ -15758,7 +15772,7 @@
       <c r="C234" t="s">
         <v>1411</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="2" t="s">
         <v>250</v>
       </c>
       <c r="E234">
@@ -15811,7 +15825,7 @@
       <c r="C235" t="s">
         <v>1411</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="2" t="s">
         <v>251</v>
       </c>
       <c r="E235">
@@ -15864,7 +15878,7 @@
       <c r="C236" t="s">
         <v>1411</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="2" t="s">
         <v>252</v>
       </c>
       <c r="E236">
@@ -15917,7 +15931,7 @@
       <c r="C237" t="s">
         <v>1411</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="2" t="s">
         <v>253</v>
       </c>
       <c r="E237">
@@ -15970,7 +15984,7 @@
       <c r="C238" t="s">
         <v>1411</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="2" t="s">
         <v>254</v>
       </c>
       <c r="E238">
@@ -16023,7 +16037,7 @@
       <c r="C239" t="s">
         <v>1411</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="2" t="s">
         <v>255</v>
       </c>
       <c r="E239">
@@ -16076,7 +16090,7 @@
       <c r="C240" t="s">
         <v>1411</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="2" t="s">
         <v>256</v>
       </c>
       <c r="E240">
@@ -16129,7 +16143,7 @@
       <c r="C241" t="s">
         <v>1411</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E241">
@@ -16182,7 +16196,7 @@
       <c r="C242" t="s">
         <v>1411</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E242">
@@ -16235,7 +16249,7 @@
       <c r="C243" t="s">
         <v>1411</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="3" t="s">
         <v>259</v>
       </c>
       <c r="E243">
@@ -16288,7 +16302,7 @@
       <c r="C244" t="s">
         <v>1411</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="3" t="s">
         <v>260</v>
       </c>
       <c r="E244">
@@ -16341,7 +16355,7 @@
       <c r="C245" t="s">
         <v>1411</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="3" t="s">
         <v>261</v>
       </c>
       <c r="E245">
@@ -16394,7 +16408,7 @@
       <c r="C246" t="s">
         <v>1411</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D246" s="3" t="s">
         <v>262</v>
       </c>
       <c r="E246">
@@ -16447,7 +16461,7 @@
       <c r="C247" t="s">
         <v>1411</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="3" t="s">
         <v>263</v>
       </c>
       <c r="E247">
@@ -16500,7 +16514,7 @@
       <c r="C248" t="s">
         <v>1411</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="3" t="s">
         <v>264</v>
       </c>
       <c r="E248">
@@ -16553,7 +16567,7 @@
       <c r="C249" t="s">
         <v>1411</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="3" t="s">
         <v>265</v>
       </c>
       <c r="E249">
@@ -16606,7 +16620,7 @@
       <c r="C250" t="s">
         <v>1411</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="3" t="s">
         <v>266</v>
       </c>
       <c r="E250">
@@ -16659,7 +16673,7 @@
       <c r="C251" t="s">
         <v>1411</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D251" s="2" t="s">
         <v>267</v>
       </c>
       <c r="E251">
@@ -16712,7 +16726,7 @@
       <c r="C252" t="s">
         <v>1411</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D252" s="2" t="s">
         <v>268</v>
       </c>
       <c r="E252">
@@ -16765,7 +16779,7 @@
       <c r="C253" t="s">
         <v>1411</v>
       </c>
-      <c r="D253" t="s">
+      <c r="D253" s="2" t="s">
         <v>269</v>
       </c>
       <c r="E253">
@@ -16818,7 +16832,7 @@
       <c r="C254" t="s">
         <v>1411</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D254" s="2" t="s">
         <v>270</v>
       </c>
       <c r="E254">
@@ -16871,7 +16885,7 @@
       <c r="C255" t="s">
         <v>1411</v>
       </c>
-      <c r="D255" t="s">
+      <c r="D255" s="2" t="s">
         <v>271</v>
       </c>
       <c r="E255">
@@ -16924,7 +16938,7 @@
       <c r="C256" t="s">
         <v>1411</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D256" s="2" t="s">
         <v>272</v>
       </c>
       <c r="E256">
@@ -16977,7 +16991,7 @@
       <c r="C257" t="s">
         <v>1411</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="2" t="s">
         <v>273</v>
       </c>
       <c r="E257">
@@ -17030,7 +17044,7 @@
       <c r="C258" t="s">
         <v>1411</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="2" t="s">
         <v>274</v>
       </c>
       <c r="E258">
@@ -17083,7 +17097,7 @@
       <c r="C259" t="s">
         <v>1411</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" s="2" t="s">
         <v>275</v>
       </c>
       <c r="E259">
@@ -17136,7 +17150,7 @@
       <c r="C260" t="s">
         <v>1411</v>
       </c>
-      <c r="D260" t="s">
+      <c r="D260" s="2" t="s">
         <v>276</v>
       </c>
       <c r="E260">
@@ -17189,7 +17203,7 @@
       <c r="C261" t="s">
         <v>1411</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="2" t="s">
         <v>277</v>
       </c>
       <c r="E261">
@@ -17242,7 +17256,7 @@
       <c r="C262" t="s">
         <v>1411</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="2" t="s">
         <v>278</v>
       </c>
       <c r="E262">
@@ -17295,7 +17309,7 @@
       <c r="C263" t="s">
         <v>1411</v>
       </c>
-      <c r="D263" t="s">
+      <c r="D263" s="2" t="s">
         <v>279</v>
       </c>
       <c r="E263">
@@ -17348,7 +17362,7 @@
       <c r="C264" t="s">
         <v>1411</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D264" s="2" t="s">
         <v>280</v>
       </c>
       <c r="E264">
@@ -17401,7 +17415,7 @@
       <c r="C265" t="s">
         <v>1411</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D265" s="2" t="s">
         <v>281</v>
       </c>
       <c r="E265">
@@ -17454,7 +17468,7 @@
       <c r="C266" t="s">
         <v>1411</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="2" t="s">
         <v>282</v>
       </c>
       <c r="E266">
@@ -17507,7 +17521,7 @@
       <c r="C267" t="s">
         <v>1411</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D267" s="2" t="s">
         <v>283</v>
       </c>
       <c r="E267">
@@ -17560,7 +17574,7 @@
       <c r="C268" t="s">
         <v>1411</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D268" s="2" t="s">
         <v>284</v>
       </c>
       <c r="E268">
@@ -17613,7 +17627,7 @@
       <c r="C269" t="s">
         <v>1411</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="2" t="s">
         <v>285</v>
       </c>
       <c r="E269">
@@ -17666,7 +17680,7 @@
       <c r="C270" t="s">
         <v>1411</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D270" s="2" t="s">
         <v>286</v>
       </c>
       <c r="E270">
@@ -17719,7 +17733,7 @@
       <c r="C271" t="s">
         <v>1411</v>
       </c>
-      <c r="D271" t="s">
+      <c r="D271" s="2" t="s">
         <v>287</v>
       </c>
       <c r="E271">
@@ -17772,7 +17786,7 @@
       <c r="C272" t="s">
         <v>1411</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="2" t="s">
         <v>288</v>
       </c>
       <c r="E272">
@@ -17825,7 +17839,7 @@
       <c r="C273" t="s">
         <v>1411</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="2" t="s">
         <v>289</v>
       </c>
       <c r="E273">
@@ -17878,7 +17892,7 @@
       <c r="C274" t="s">
         <v>1411</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D274" s="2" t="s">
         <v>290</v>
       </c>
       <c r="E274">
@@ -17931,7 +17945,7 @@
       <c r="C275" t="s">
         <v>1411</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="2" t="s">
         <v>291</v>
       </c>
       <c r="E275">
@@ -17984,7 +17998,7 @@
       <c r="C276" t="s">
         <v>1411</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="2" t="s">
         <v>292</v>
       </c>
       <c r="E276">
@@ -18037,7 +18051,7 @@
       <c r="C277" t="s">
         <v>1411</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="2" t="s">
         <v>293</v>
       </c>
       <c r="E277">
@@ -18090,7 +18104,7 @@
       <c r="C278" t="s">
         <v>1411</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="2" t="s">
         <v>294</v>
       </c>
       <c r="E278">
@@ -18143,7 +18157,7 @@
       <c r="C279" t="s">
         <v>1411</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="2" t="s">
         <v>295</v>
       </c>
       <c r="E279">
@@ -18196,7 +18210,7 @@
       <c r="C280" t="s">
         <v>1411</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="2" t="s">
         <v>296</v>
       </c>
       <c r="E280">
@@ -18249,7 +18263,7 @@
       <c r="C281" t="s">
         <v>1411</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="3" t="s">
         <v>297</v>
       </c>
       <c r="E281">
@@ -18302,7 +18316,7 @@
       <c r="C282" t="s">
         <v>1411</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="3" t="s">
         <v>298</v>
       </c>
       <c r="E282">
@@ -18355,7 +18369,7 @@
       <c r="C283" t="s">
         <v>1411</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="3" t="s">
         <v>299</v>
       </c>
       <c r="E283">
@@ -18408,7 +18422,7 @@
       <c r="C284" t="s">
         <v>1411</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="3" t="s">
         <v>300</v>
       </c>
       <c r="E284">
@@ -18461,7 +18475,7 @@
       <c r="C285" t="s">
         <v>1411</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E285">
@@ -18514,7 +18528,7 @@
       <c r="C286" t="s">
         <v>1411</v>
       </c>
-      <c r="D286" t="s">
+      <c r="D286" s="3" t="s">
         <v>302</v>
       </c>
       <c r="E286">
@@ -18567,7 +18581,7 @@
       <c r="C287" t="s">
         <v>1411</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="3" t="s">
         <v>303</v>
       </c>
       <c r="E287">
@@ -18620,7 +18634,7 @@
       <c r="C288" t="s">
         <v>1411</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D288" s="3" t="s">
         <v>304</v>
       </c>
       <c r="E288">
@@ -18673,7 +18687,7 @@
       <c r="C289" t="s">
         <v>1411</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D289" s="3" t="s">
         <v>305</v>
       </c>
       <c r="E289">
@@ -18726,7 +18740,7 @@
       <c r="C290" t="s">
         <v>1411</v>
       </c>
-      <c r="D290" t="s">
+      <c r="D290" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E290">
@@ -18779,7 +18793,7 @@
       <c r="C291" t="s">
         <v>1411</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="2" t="s">
         <v>307</v>
       </c>
       <c r="E291">
@@ -18832,7 +18846,7 @@
       <c r="C292" t="s">
         <v>1411</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D292" s="2" t="s">
         <v>308</v>
       </c>
       <c r="E292">
@@ -18885,7 +18899,7 @@
       <c r="C293" t="s">
         <v>1411</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D293" s="2" t="s">
         <v>309</v>
       </c>
       <c r="E293">
@@ -18938,7 +18952,7 @@
       <c r="C294" t="s">
         <v>1411</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D294" s="2" t="s">
         <v>310</v>
       </c>
       <c r="E294">
@@ -18991,7 +19005,7 @@
       <c r="C295" t="s">
         <v>1411</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D295" s="2" t="s">
         <v>311</v>
       </c>
       <c r="E295">
@@ -19044,7 +19058,7 @@
       <c r="C296" t="s">
         <v>1411</v>
       </c>
-      <c r="D296" t="s">
+      <c r="D296" s="2" t="s">
         <v>312</v>
       </c>
       <c r="E296">
@@ -19097,7 +19111,7 @@
       <c r="C297" t="s">
         <v>1411</v>
       </c>
-      <c r="D297" t="s">
+      <c r="D297" s="2" t="s">
         <v>313</v>
       </c>
       <c r="E297">
@@ -19150,7 +19164,7 @@
       <c r="C298" t="s">
         <v>1411</v>
       </c>
-      <c r="D298" t="s">
+      <c r="D298" s="2" t="s">
         <v>314</v>
       </c>
       <c r="E298">
@@ -19203,7 +19217,7 @@
       <c r="C299" t="s">
         <v>1411</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E299">
@@ -19256,7 +19270,7 @@
       <c r="C300" t="s">
         <v>1411</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D300" s="2" t="s">
         <v>316</v>
       </c>
       <c r="E300">
@@ -19309,7 +19323,7 @@
       <c r="C301" t="s">
         <v>1411</v>
       </c>
-      <c r="D301" t="s">
+      <c r="D301" s="2" t="s">
         <v>317</v>
       </c>
       <c r="E301">
@@ -19362,7 +19376,7 @@
       <c r="C302" t="s">
         <v>1411</v>
       </c>
-      <c r="D302" t="s">
+      <c r="D302" s="2" t="s">
         <v>318</v>
       </c>
       <c r="E302">
@@ -19415,7 +19429,7 @@
       <c r="C303" t="s">
         <v>1411</v>
       </c>
-      <c r="D303" t="s">
+      <c r="D303" s="2" t="s">
         <v>319</v>
       </c>
       <c r="E303">
@@ -19468,7 +19482,7 @@
       <c r="C304" t="s">
         <v>1411</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D304" s="2" t="s">
         <v>320</v>
       </c>
       <c r="E304">
@@ -19521,7 +19535,7 @@
       <c r="C305" t="s">
         <v>1411</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D305" s="2" t="s">
         <v>321</v>
       </c>
       <c r="E305">
@@ -19574,7 +19588,7 @@
       <c r="C306" t="s">
         <v>1411</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D306" s="2" t="s">
         <v>322</v>
       </c>
       <c r="E306">
@@ -19627,7 +19641,7 @@
       <c r="C307" t="s">
         <v>1411</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D307" s="2" t="s">
         <v>323</v>
       </c>
       <c r="E307">
@@ -19680,7 +19694,7 @@
       <c r="C308" t="s">
         <v>1411</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D308" s="2" t="s">
         <v>324</v>
       </c>
       <c r="E308">
@@ -19733,7 +19747,7 @@
       <c r="C309" t="s">
         <v>1411</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" s="2" t="s">
         <v>325</v>
       </c>
       <c r="E309">
@@ -19786,7 +19800,7 @@
       <c r="C310" t="s">
         <v>1411</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D310" s="2" t="s">
         <v>326</v>
       </c>
       <c r="E310">
@@ -19839,7 +19853,7 @@
       <c r="C311" t="s">
         <v>1411</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D311" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E311">
@@ -19892,7 +19906,7 @@
       <c r="C312" t="s">
         <v>1411</v>
       </c>
-      <c r="D312" t="s">
+      <c r="D312" s="2" t="s">
         <v>328</v>
       </c>
       <c r="E312">
@@ -19945,7 +19959,7 @@
       <c r="C313" t="s">
         <v>1411</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D313" s="2" t="s">
         <v>329</v>
       </c>
       <c r="E313">
@@ -19998,7 +20012,7 @@
       <c r="C314" t="s">
         <v>1411</v>
       </c>
-      <c r="D314" t="s">
+      <c r="D314" s="2" t="s">
         <v>330</v>
       </c>
       <c r="E314">
@@ -20051,7 +20065,7 @@
       <c r="C315" t="s">
         <v>1411</v>
       </c>
-      <c r="D315" t="s">
+      <c r="D315" s="2" t="s">
         <v>331</v>
       </c>
       <c r="E315">
@@ -20104,7 +20118,7 @@
       <c r="C316" t="s">
         <v>1411</v>
       </c>
-      <c r="D316" t="s">
+      <c r="D316" s="2" t="s">
         <v>332</v>
       </c>
       <c r="E316">
@@ -20157,7 +20171,7 @@
       <c r="C317" t="s">
         <v>1411</v>
       </c>
-      <c r="D317" t="s">
+      <c r="D317" s="2" t="s">
         <v>333</v>
       </c>
       <c r="E317">
@@ -20210,7 +20224,7 @@
       <c r="C318" t="s">
         <v>1411</v>
       </c>
-      <c r="D318" t="s">
+      <c r="D318" s="2" t="s">
         <v>334</v>
       </c>
       <c r="E318">
@@ -20263,7 +20277,7 @@
       <c r="C319" t="s">
         <v>1411</v>
       </c>
-      <c r="D319" t="s">
+      <c r="D319" s="2" t="s">
         <v>335</v>
       </c>
       <c r="E319">
@@ -20316,7 +20330,7 @@
       <c r="C320" t="s">
         <v>1411</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D320" s="2" t="s">
         <v>336</v>
       </c>
       <c r="E320">
@@ -20369,7 +20383,7 @@
       <c r="C321" t="s">
         <v>1411</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D321" s="3" t="s">
         <v>337</v>
       </c>
       <c r="E321">
@@ -20422,7 +20436,7 @@
       <c r="C322" t="s">
         <v>1411</v>
       </c>
-      <c r="D322" t="s">
+      <c r="D322" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E322">
@@ -20475,7 +20489,7 @@
       <c r="C323" t="s">
         <v>1411</v>
       </c>
-      <c r="D323" t="s">
+      <c r="D323" s="3" t="s">
         <v>339</v>
       </c>
       <c r="E323">
@@ -20528,7 +20542,7 @@
       <c r="C324" t="s">
         <v>1411</v>
       </c>
-      <c r="D324" t="s">
+      <c r="D324" s="3" t="s">
         <v>340</v>
       </c>
       <c r="E324">
@@ -20581,7 +20595,7 @@
       <c r="C325" t="s">
         <v>1411</v>
       </c>
-      <c r="D325" t="s">
+      <c r="D325" s="3" t="s">
         <v>341</v>
       </c>
       <c r="E325">
@@ -20634,7 +20648,7 @@
       <c r="C326" t="s">
         <v>1411</v>
       </c>
-      <c r="D326" t="s">
+      <c r="D326" s="3" t="s">
         <v>342</v>
       </c>
       <c r="E326">
@@ -20687,7 +20701,7 @@
       <c r="C327" t="s">
         <v>1411</v>
       </c>
-      <c r="D327" t="s">
+      <c r="D327" s="3" t="s">
         <v>343</v>
       </c>
       <c r="E327">
@@ -20740,7 +20754,7 @@
       <c r="C328" t="s">
         <v>1411</v>
       </c>
-      <c r="D328" t="s">
+      <c r="D328" s="3" t="s">
         <v>344</v>
       </c>
       <c r="E328">
@@ -20793,7 +20807,7 @@
       <c r="C329" t="s">
         <v>1411</v>
       </c>
-      <c r="D329" t="s">
+      <c r="D329" s="3" t="s">
         <v>345</v>
       </c>
       <c r="E329">
@@ -20846,7 +20860,7 @@
       <c r="C330" t="s">
         <v>1411</v>
       </c>
-      <c r="D330" t="s">
+      <c r="D330" s="3" t="s">
         <v>346</v>
       </c>
       <c r="E330">
@@ -20899,7 +20913,7 @@
       <c r="C331" t="s">
         <v>1411</v>
       </c>
-      <c r="D331" t="s">
+      <c r="D331" s="2" t="s">
         <v>347</v>
       </c>
       <c r="E331">
@@ -20952,7 +20966,7 @@
       <c r="C332" t="s">
         <v>1411</v>
       </c>
-      <c r="D332" t="s">
+      <c r="D332" s="2" t="s">
         <v>348</v>
       </c>
       <c r="E332">
@@ -21005,7 +21019,7 @@
       <c r="C333" t="s">
         <v>1411</v>
       </c>
-      <c r="D333" t="s">
+      <c r="D333" s="2" t="s">
         <v>349</v>
       </c>
       <c r="E333">
@@ -21058,7 +21072,7 @@
       <c r="C334" t="s">
         <v>1411</v>
       </c>
-      <c r="D334" t="s">
+      <c r="D334" s="2" t="s">
         <v>350</v>
       </c>
       <c r="E334">
@@ -21111,7 +21125,7 @@
       <c r="C335" t="s">
         <v>1411</v>
       </c>
-      <c r="D335" t="s">
+      <c r="D335" s="2" t="s">
         <v>351</v>
       </c>
       <c r="E335">
@@ -21164,7 +21178,7 @@
       <c r="C336" t="s">
         <v>1411</v>
       </c>
-      <c r="D336" t="s">
+      <c r="D336" s="2" t="s">
         <v>352</v>
       </c>
       <c r="E336">
@@ -21217,7 +21231,7 @@
       <c r="C337" t="s">
         <v>1411</v>
       </c>
-      <c r="D337" t="s">
+      <c r="D337" s="2" t="s">
         <v>353</v>
       </c>
       <c r="E337">
@@ -21270,7 +21284,7 @@
       <c r="C338" t="s">
         <v>1411</v>
       </c>
-      <c r="D338" t="s">
+      <c r="D338" s="2" t="s">
         <v>354</v>
       </c>
       <c r="E338">
@@ -21323,7 +21337,7 @@
       <c r="C339" t="s">
         <v>1411</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D339" s="2" t="s">
         <v>355</v>
       </c>
       <c r="E339">
@@ -21376,7 +21390,7 @@
       <c r="C340" t="s">
         <v>1411</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D340" s="2" t="s">
         <v>356</v>
       </c>
       <c r="E340">
@@ -21429,7 +21443,7 @@
       <c r="C341" t="s">
         <v>1411</v>
       </c>
-      <c r="D341" t="s">
+      <c r="D341" s="2" t="s">
         <v>357</v>
       </c>
       <c r="E341">
@@ -21482,7 +21496,7 @@
       <c r="C342" t="s">
         <v>1411</v>
       </c>
-      <c r="D342" t="s">
+      <c r="D342" s="2" t="s">
         <v>358</v>
       </c>
       <c r="E342">
@@ -21535,7 +21549,7 @@
       <c r="C343" t="s">
         <v>1411</v>
       </c>
-      <c r="D343" t="s">
+      <c r="D343" s="2" t="s">
         <v>359</v>
       </c>
       <c r="E343">
@@ -21588,7 +21602,7 @@
       <c r="C344" t="s">
         <v>1411</v>
       </c>
-      <c r="D344" t="s">
+      <c r="D344" s="2" t="s">
         <v>360</v>
       </c>
       <c r="E344">
@@ -21641,7 +21655,7 @@
       <c r="C345" t="s">
         <v>1411</v>
       </c>
-      <c r="D345" t="s">
+      <c r="D345" s="2" t="s">
         <v>361</v>
       </c>
       <c r="E345">
@@ -21694,7 +21708,7 @@
       <c r="C346" t="s">
         <v>1411</v>
       </c>
-      <c r="D346" t="s">
+      <c r="D346" s="2" t="s">
         <v>362</v>
       </c>
       <c r="E346">
@@ -21747,7 +21761,7 @@
       <c r="C347" t="s">
         <v>1411</v>
       </c>
-      <c r="D347" t="s">
+      <c r="D347" s="2" t="s">
         <v>363</v>
       </c>
       <c r="E347">
@@ -21800,7 +21814,7 @@
       <c r="C348" t="s">
         <v>1411</v>
       </c>
-      <c r="D348" t="s">
+      <c r="D348" s="2" t="s">
         <v>364</v>
       </c>
       <c r="E348">
@@ -21853,7 +21867,7 @@
       <c r="C349" t="s">
         <v>1411</v>
       </c>
-      <c r="D349" t="s">
+      <c r="D349" s="2" t="s">
         <v>365</v>
       </c>
       <c r="E349">
@@ -21906,7 +21920,7 @@
       <c r="C350" t="s">
         <v>1411</v>
       </c>
-      <c r="D350" t="s">
+      <c r="D350" s="2" t="s">
         <v>366</v>
       </c>
       <c r="E350">
@@ -21959,7 +21973,7 @@
       <c r="C351" t="s">
         <v>1411</v>
       </c>
-      <c r="D351" t="s">
+      <c r="D351" s="2" t="s">
         <v>367</v>
       </c>
       <c r="E351">
@@ -22012,7 +22026,7 @@
       <c r="C352" t="s">
         <v>1411</v>
       </c>
-      <c r="D352" t="s">
+      <c r="D352" s="2" t="s">
         <v>368</v>
       </c>
       <c r="E352">
@@ -22065,7 +22079,7 @@
       <c r="C353" t="s">
         <v>1411</v>
       </c>
-      <c r="D353" t="s">
+      <c r="D353" s="2" t="s">
         <v>369</v>
       </c>
       <c r="E353">
@@ -22118,7 +22132,7 @@
       <c r="C354" t="s">
         <v>1411</v>
       </c>
-      <c r="D354" t="s">
+      <c r="D354" s="2" t="s">
         <v>370</v>
       </c>
       <c r="E354">
@@ -22171,7 +22185,7 @@
       <c r="C355" t="s">
         <v>1411</v>
       </c>
-      <c r="D355" t="s">
+      <c r="D355" s="2" t="s">
         <v>371</v>
       </c>
       <c r="E355">
@@ -22224,7 +22238,7 @@
       <c r="C356" t="s">
         <v>1411</v>
       </c>
-      <c r="D356" t="s">
+      <c r="D356" s="2" t="s">
         <v>372</v>
       </c>
       <c r="E356">
@@ -22277,7 +22291,7 @@
       <c r="C357" t="s">
         <v>1411</v>
       </c>
-      <c r="D357" t="s">
+      <c r="D357" s="2" t="s">
         <v>373</v>
       </c>
       <c r="E357">
@@ -22330,7 +22344,7 @@
       <c r="C358" t="s">
         <v>1411</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D358" s="2" t="s">
         <v>374</v>
       </c>
       <c r="E358">
@@ -22383,7 +22397,7 @@
       <c r="C359" t="s">
         <v>1411</v>
       </c>
-      <c r="D359" t="s">
+      <c r="D359" s="2" t="s">
         <v>375</v>
       </c>
       <c r="E359">
@@ -22436,7 +22450,7 @@
       <c r="C360" t="s">
         <v>1411</v>
       </c>
-      <c r="D360" t="s">
+      <c r="D360" s="2" t="s">
         <v>376</v>
       </c>
       <c r="E360">
@@ -22489,7 +22503,7 @@
       <c r="C361" t="s">
         <v>1411</v>
       </c>
-      <c r="D361" t="s">
+      <c r="D361" s="3" t="s">
         <v>377</v>
       </c>
       <c r="E361">
@@ -22542,7 +22556,7 @@
       <c r="C362" t="s">
         <v>1411</v>
       </c>
-      <c r="D362" t="s">
+      <c r="D362" s="3" t="s">
         <v>378</v>
       </c>
       <c r="E362">
@@ -22595,7 +22609,7 @@
       <c r="C363" t="s">
         <v>1411</v>
       </c>
-      <c r="D363" t="s">
+      <c r="D363" s="3" t="s">
         <v>379</v>
       </c>
       <c r="E363">
@@ -22648,7 +22662,7 @@
       <c r="C364" t="s">
         <v>1411</v>
       </c>
-      <c r="D364" t="s">
+      <c r="D364" s="3" t="s">
         <v>380</v>
       </c>
       <c r="E364">
@@ -22701,7 +22715,7 @@
       <c r="C365" t="s">
         <v>1411</v>
       </c>
-      <c r="D365" t="s">
+      <c r="D365" s="3" t="s">
         <v>381</v>
       </c>
       <c r="E365">
@@ -22754,7 +22768,7 @@
       <c r="C366" t="s">
         <v>1411</v>
       </c>
-      <c r="D366" t="s">
+      <c r="D366" s="3" t="s">
         <v>382</v>
       </c>
       <c r="E366">
@@ -22807,7 +22821,7 @@
       <c r="C367" t="s">
         <v>1411</v>
       </c>
-      <c r="D367" t="s">
+      <c r="D367" s="3" t="s">
         <v>383</v>
       </c>
       <c r="E367">
@@ -22860,7 +22874,7 @@
       <c r="C368" t="s">
         <v>1411</v>
       </c>
-      <c r="D368" t="s">
+      <c r="D368" s="3" t="s">
         <v>384</v>
       </c>
       <c r="E368">
@@ -22913,7 +22927,7 @@
       <c r="C369" t="s">
         <v>1411</v>
       </c>
-      <c r="D369" t="s">
+      <c r="D369" s="3" t="s">
         <v>385</v>
       </c>
       <c r="E369">
@@ -22966,7 +22980,7 @@
       <c r="C370" t="s">
         <v>1411</v>
       </c>
-      <c r="D370" t="s">
+      <c r="D370" s="3" t="s">
         <v>386</v>
       </c>
       <c r="E370">
@@ -23019,7 +23033,7 @@
       <c r="C371" t="s">
         <v>1411</v>
       </c>
-      <c r="D371" t="s">
+      <c r="D371" s="2" t="s">
         <v>387</v>
       </c>
       <c r="E371">
@@ -23072,7 +23086,7 @@
       <c r="C372" t="s">
         <v>1411</v>
       </c>
-      <c r="D372" t="s">
+      <c r="D372" s="2" t="s">
         <v>388</v>
       </c>
       <c r="E372">
@@ -23125,7 +23139,7 @@
       <c r="C373" t="s">
         <v>1411</v>
       </c>
-      <c r="D373" t="s">
+      <c r="D373" s="2" t="s">
         <v>389</v>
       </c>
       <c r="E373">
@@ -23178,7 +23192,7 @@
       <c r="C374" t="s">
         <v>1411</v>
       </c>
-      <c r="D374" t="s">
+      <c r="D374" s="2" t="s">
         <v>390</v>
       </c>
       <c r="E374">
@@ -23231,7 +23245,7 @@
       <c r="C375" t="s">
         <v>1411</v>
       </c>
-      <c r="D375" t="s">
+      <c r="D375" s="2" t="s">
         <v>391</v>
       </c>
       <c r="E375">
@@ -23284,7 +23298,7 @@
       <c r="C376" t="s">
         <v>1411</v>
       </c>
-      <c r="D376" t="s">
+      <c r="D376" s="2" t="s">
         <v>392</v>
       </c>
       <c r="E376">
@@ -23337,7 +23351,7 @@
       <c r="C377" t="s">
         <v>1411</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D377" s="2" t="s">
         <v>393</v>
       </c>
       <c r="E377">
@@ -23390,7 +23404,7 @@
       <c r="C378" t="s">
         <v>1411</v>
       </c>
-      <c r="D378" t="s">
+      <c r="D378" s="2" t="s">
         <v>394</v>
       </c>
       <c r="E378">
@@ -23443,7 +23457,7 @@
       <c r="C379" t="s">
         <v>1411</v>
       </c>
-      <c r="D379" t="s">
+      <c r="D379" s="2" t="s">
         <v>395</v>
       </c>
       <c r="E379">
@@ -23496,7 +23510,7 @@
       <c r="C380" t="s">
         <v>1411</v>
       </c>
-      <c r="D380" t="s">
+      <c r="D380" s="2" t="s">
         <v>396</v>
       </c>
       <c r="E380">
@@ -23549,7 +23563,7 @@
       <c r="C381" t="s">
         <v>1411</v>
       </c>
-      <c r="D381" t="s">
+      <c r="D381" s="2" t="s">
         <v>397</v>
       </c>
       <c r="E381">
@@ -23602,7 +23616,7 @@
       <c r="C382" t="s">
         <v>1411</v>
       </c>
-      <c r="D382" t="s">
+      <c r="D382" s="2" t="s">
         <v>398</v>
       </c>
       <c r="E382">
@@ -23655,7 +23669,7 @@
       <c r="C383" t="s">
         <v>1411</v>
       </c>
-      <c r="D383" t="s">
+      <c r="D383" s="2" t="s">
         <v>399</v>
       </c>
       <c r="E383">
@@ -23708,7 +23722,7 @@
       <c r="C384" t="s">
         <v>1411</v>
       </c>
-      <c r="D384" t="s">
+      <c r="D384" s="2" t="s">
         <v>400</v>
       </c>
       <c r="E384">
@@ -23761,7 +23775,7 @@
       <c r="C385" t="s">
         <v>1411</v>
       </c>
-      <c r="D385" t="s">
+      <c r="D385" s="2" t="s">
         <v>401</v>
       </c>
       <c r="E385">
@@ -23814,7 +23828,7 @@
       <c r="C386" t="s">
         <v>1411</v>
       </c>
-      <c r="D386" t="s">
+      <c r="D386" s="2" t="s">
         <v>402</v>
       </c>
       <c r="E386">
@@ -23867,7 +23881,7 @@
       <c r="C387" t="s">
         <v>1411</v>
       </c>
-      <c r="D387" t="s">
+      <c r="D387" s="2" t="s">
         <v>403</v>
       </c>
       <c r="E387">
@@ -23920,7 +23934,7 @@
       <c r="C388" t="s">
         <v>1411</v>
       </c>
-      <c r="D388" t="s">
+      <c r="D388" s="2" t="s">
         <v>404</v>
       </c>
       <c r="E388">
@@ -23973,7 +23987,7 @@
       <c r="C389" t="s">
         <v>1411</v>
       </c>
-      <c r="D389" t="s">
+      <c r="D389" s="2" t="s">
         <v>405</v>
       </c>
       <c r="E389">
@@ -24026,7 +24040,7 @@
       <c r="C390" t="s">
         <v>1411</v>
       </c>
-      <c r="D390" t="s">
+      <c r="D390" s="2" t="s">
         <v>406</v>
       </c>
       <c r="E390">
@@ -24079,7 +24093,7 @@
       <c r="C391" t="s">
         <v>1411</v>
       </c>
-      <c r="D391" t="s">
+      <c r="D391" s="2" t="s">
         <v>407</v>
       </c>
       <c r="E391">
@@ -24132,7 +24146,7 @@
       <c r="C392" t="s">
         <v>1411</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D392" s="2" t="s">
         <v>408</v>
       </c>
       <c r="E392">
@@ -24185,7 +24199,7 @@
       <c r="C393" t="s">
         <v>1411</v>
       </c>
-      <c r="D393" t="s">
+      <c r="D393" s="2" t="s">
         <v>409</v>
       </c>
       <c r="E393">
@@ -24238,7 +24252,7 @@
       <c r="C394" t="s">
         <v>1411</v>
       </c>
-      <c r="D394" t="s">
+      <c r="D394" s="2" t="s">
         <v>410</v>
       </c>
       <c r="E394">
@@ -24291,7 +24305,7 @@
       <c r="C395" t="s">
         <v>1411</v>
       </c>
-      <c r="D395" t="s">
+      <c r="D395" s="2" t="s">
         <v>411</v>
       </c>
       <c r="E395">
@@ -24344,7 +24358,7 @@
       <c r="C396" t="s">
         <v>1411</v>
       </c>
-      <c r="D396" t="s">
+      <c r="D396" s="2" t="s">
         <v>412</v>
       </c>
       <c r="E396">
@@ -24397,7 +24411,7 @@
       <c r="C397" t="s">
         <v>1411</v>
       </c>
-      <c r="D397" t="s">
+      <c r="D397" s="2" t="s">
         <v>413</v>
       </c>
       <c r="E397">
@@ -24450,7 +24464,7 @@
       <c r="C398" t="s">
         <v>1411</v>
       </c>
-      <c r="D398" t="s">
+      <c r="D398" s="2" t="s">
         <v>414</v>
       </c>
       <c r="E398">
@@ -24503,7 +24517,7 @@
       <c r="C399" t="s">
         <v>1411</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D399" s="2" t="s">
         <v>415</v>
       </c>
       <c r="E399">
@@ -24556,7 +24570,7 @@
       <c r="C400" t="s">
         <v>1411</v>
       </c>
-      <c r="D400" t="s">
+      <c r="D400" s="2" t="s">
         <v>416</v>
       </c>
       <c r="E400">
@@ -24609,7 +24623,7 @@
       <c r="C401" t="s">
         <v>1411</v>
       </c>
-      <c r="D401" t="s">
+      <c r="D401" s="3" t="s">
         <v>417</v>
       </c>
       <c r="E401">
@@ -24662,7 +24676,7 @@
       <c r="C402" t="s">
         <v>1411</v>
       </c>
-      <c r="D402" t="s">
+      <c r="D402" s="3" t="s">
         <v>418</v>
       </c>
       <c r="E402">
@@ -24715,7 +24729,7 @@
       <c r="C403" t="s">
         <v>1411</v>
       </c>
-      <c r="D403" t="s">
+      <c r="D403" s="3" t="s">
         <v>419</v>
       </c>
       <c r="E403">
@@ -24768,7 +24782,7 @@
       <c r="C404" t="s">
         <v>1411</v>
       </c>
-      <c r="D404" t="s">
+      <c r="D404" s="3" t="s">
         <v>420</v>
       </c>
       <c r="E404">
@@ -24821,7 +24835,7 @@
       <c r="C405" t="s">
         <v>1411</v>
       </c>
-      <c r="D405" t="s">
+      <c r="D405" s="3" t="s">
         <v>421</v>
       </c>
       <c r="E405">
@@ -24874,7 +24888,7 @@
       <c r="C406" t="s">
         <v>1411</v>
       </c>
-      <c r="D406" t="s">
+      <c r="D406" s="3" t="s">
         <v>422</v>
       </c>
       <c r="E406">
@@ -24927,7 +24941,7 @@
       <c r="C407" t="s">
         <v>1411</v>
       </c>
-      <c r="D407" t="s">
+      <c r="D407" s="3" t="s">
         <v>423</v>
       </c>
       <c r="E407">
@@ -24980,7 +24994,7 @@
       <c r="C408" t="s">
         <v>1411</v>
       </c>
-      <c r="D408" t="s">
+      <c r="D408" s="3" t="s">
         <v>424</v>
       </c>
       <c r="E408">
@@ -25033,7 +25047,7 @@
       <c r="C409" t="s">
         <v>1411</v>
       </c>
-      <c r="D409" t="s">
+      <c r="D409" s="3" t="s">
         <v>425</v>
       </c>
       <c r="E409">
@@ -25086,7 +25100,7 @@
       <c r="C410" t="s">
         <v>1411</v>
       </c>
-      <c r="D410" t="s">
+      <c r="D410" s="3" t="s">
         <v>426</v>
       </c>
       <c r="E410">
@@ -25139,7 +25153,7 @@
       <c r="C411" t="s">
         <v>1411</v>
       </c>
-      <c r="D411" t="s">
+      <c r="D411" s="2" t="s">
         <v>427</v>
       </c>
       <c r="E411">
@@ -25192,7 +25206,7 @@
       <c r="C412" t="s">
         <v>1411</v>
       </c>
-      <c r="D412" t="s">
+      <c r="D412" s="2" t="s">
         <v>428</v>
       </c>
       <c r="E412">
@@ -25245,7 +25259,7 @@
       <c r="C413" t="s">
         <v>1411</v>
       </c>
-      <c r="D413" t="s">
+      <c r="D413" s="2" t="s">
         <v>429</v>
       </c>
       <c r="E413">
@@ -25298,7 +25312,7 @@
       <c r="C414" t="s">
         <v>1411</v>
       </c>
-      <c r="D414" t="s">
+      <c r="D414" s="2" t="s">
         <v>430</v>
       </c>
       <c r="E414">
@@ -25351,7 +25365,7 @@
       <c r="C415" t="s">
         <v>1411</v>
       </c>
-      <c r="D415" t="s">
+      <c r="D415" s="2" t="s">
         <v>431</v>
       </c>
       <c r="E415">
@@ -25404,7 +25418,7 @@
       <c r="C416" t="s">
         <v>1411</v>
       </c>
-      <c r="D416" t="s">
+      <c r="D416" s="2" t="s">
         <v>432</v>
       </c>
       <c r="E416">
@@ -25457,7 +25471,7 @@
       <c r="C417" t="s">
         <v>1411</v>
       </c>
-      <c r="D417" t="s">
+      <c r="D417" s="2" t="s">
         <v>433</v>
       </c>
       <c r="E417">
@@ -25510,7 +25524,7 @@
       <c r="C418" t="s">
         <v>1411</v>
       </c>
-      <c r="D418" t="s">
+      <c r="D418" s="2" t="s">
         <v>434</v>
       </c>
       <c r="E418">
@@ -25563,7 +25577,7 @@
       <c r="C419" t="s">
         <v>1411</v>
       </c>
-      <c r="D419" t="s">
+      <c r="D419" s="2" t="s">
         <v>435</v>
       </c>
       <c r="E419">
@@ -25616,7 +25630,7 @@
       <c r="C420" t="s">
         <v>1411</v>
       </c>
-      <c r="D420" t="s">
+      <c r="D420" s="2" t="s">
         <v>436</v>
       </c>
       <c r="E420">
@@ -25669,7 +25683,7 @@
       <c r="C421" t="s">
         <v>1411</v>
       </c>
-      <c r="D421" t="s">
+      <c r="D421" s="2" t="s">
         <v>437</v>
       </c>
       <c r="E421">
@@ -25722,7 +25736,7 @@
       <c r="C422" t="s">
         <v>1411</v>
       </c>
-      <c r="D422" t="s">
+      <c r="D422" s="2" t="s">
         <v>438</v>
       </c>
       <c r="E422">
@@ -25775,7 +25789,7 @@
       <c r="C423" t="s">
         <v>1411</v>
       </c>
-      <c r="D423" t="s">
+      <c r="D423" s="2" t="s">
         <v>439</v>
       </c>
       <c r="E423">
@@ -25828,7 +25842,7 @@
       <c r="C424" t="s">
         <v>1411</v>
       </c>
-      <c r="D424" t="s">
+      <c r="D424" s="2" t="s">
         <v>440</v>
       </c>
       <c r="E424">
@@ -25881,7 +25895,7 @@
       <c r="C425" t="s">
         <v>1411</v>
       </c>
-      <c r="D425" t="s">
+      <c r="D425" s="2" t="s">
         <v>441</v>
       </c>
       <c r="E425">
@@ -25934,7 +25948,7 @@
       <c r="C426" t="s">
         <v>1411</v>
       </c>
-      <c r="D426" t="s">
+      <c r="D426" s="2" t="s">
         <v>442</v>
       </c>
       <c r="E426">
@@ -25987,7 +26001,7 @@
       <c r="C427" t="s">
         <v>1411</v>
       </c>
-      <c r="D427" t="s">
+      <c r="D427" s="2" t="s">
         <v>443</v>
       </c>
       <c r="E427">
@@ -26040,7 +26054,7 @@
       <c r="C428" t="s">
         <v>1411</v>
       </c>
-      <c r="D428" t="s">
+      <c r="D428" s="2" t="s">
         <v>444</v>
       </c>
       <c r="E428">
@@ -26093,7 +26107,7 @@
       <c r="C429" t="s">
         <v>1411</v>
       </c>
-      <c r="D429" t="s">
+      <c r="D429" s="2" t="s">
         <v>445</v>
       </c>
       <c r="E429">
@@ -26146,7 +26160,7 @@
       <c r="C430" t="s">
         <v>1411</v>
       </c>
-      <c r="D430" t="s">
+      <c r="D430" s="2" t="s">
         <v>446</v>
       </c>
       <c r="E430">
@@ -26199,7 +26213,7 @@
       <c r="C431" t="s">
         <v>1411</v>
       </c>
-      <c r="D431" t="s">
+      <c r="D431" s="2" t="s">
         <v>447</v>
       </c>
       <c r="E431">
@@ -26252,7 +26266,7 @@
       <c r="C432" t="s">
         <v>1411</v>
       </c>
-      <c r="D432" t="s">
+      <c r="D432" s="2" t="s">
         <v>448</v>
       </c>
       <c r="E432">
@@ -26305,7 +26319,7 @@
       <c r="C433" t="s">
         <v>1411</v>
       </c>
-      <c r="D433" t="s">
+      <c r="D433" s="2" t="s">
         <v>449</v>
       </c>
       <c r="E433">
@@ -26358,7 +26372,7 @@
       <c r="C434" t="s">
         <v>1411</v>
       </c>
-      <c r="D434" t="s">
+      <c r="D434" s="2" t="s">
         <v>450</v>
       </c>
       <c r="E434">
@@ -26411,7 +26425,7 @@
       <c r="C435" t="s">
         <v>1411</v>
       </c>
-      <c r="D435" t="s">
+      <c r="D435" s="2" t="s">
         <v>451</v>
       </c>
       <c r="E435">
@@ -26464,7 +26478,7 @@
       <c r="C436" t="s">
         <v>1411</v>
       </c>
-      <c r="D436" t="s">
+      <c r="D436" s="2" t="s">
         <v>452</v>
       </c>
       <c r="E436">
@@ -26517,7 +26531,7 @@
       <c r="C437" t="s">
         <v>1411</v>
       </c>
-      <c r="D437" t="s">
+      <c r="D437" s="2" t="s">
         <v>453</v>
       </c>
       <c r="E437">
@@ -26570,7 +26584,7 @@
       <c r="C438" t="s">
         <v>1411</v>
       </c>
-      <c r="D438" t="s">
+      <c r="D438" s="2" t="s">
         <v>454</v>
       </c>
       <c r="E438">
@@ -26623,7 +26637,7 @@
       <c r="C439" t="s">
         <v>1411</v>
       </c>
-      <c r="D439" t="s">
+      <c r="D439" s="2" t="s">
         <v>455</v>
       </c>
       <c r="E439">
@@ -26676,7 +26690,7 @@
       <c r="C440" t="s">
         <v>1411</v>
       </c>
-      <c r="D440" t="s">
+      <c r="D440" s="2" t="s">
         <v>456</v>
       </c>
       <c r="E440">
@@ -26729,7 +26743,7 @@
       <c r="C441" t="s">
         <v>1411</v>
       </c>
-      <c r="D441" t="s">
+      <c r="D441" s="3" t="s">
         <v>457</v>
       </c>
       <c r="E441">
@@ -26782,7 +26796,7 @@
       <c r="C442" t="s">
         <v>1411</v>
       </c>
-      <c r="D442" t="s">
+      <c r="D442" s="3" t="s">
         <v>458</v>
       </c>
       <c r="E442">
@@ -26835,7 +26849,7 @@
       <c r="C443" t="s">
         <v>1411</v>
       </c>
-      <c r="D443" t="s">
+      <c r="D443" s="3" t="s">
         <v>459</v>
       </c>
       <c r="E443">
@@ -26888,7 +26902,7 @@
       <c r="C444" t="s">
         <v>1411</v>
       </c>
-      <c r="D444" t="s">
+      <c r="D444" s="3" t="s">
         <v>460</v>
       </c>
       <c r="E444">
@@ -26941,7 +26955,7 @@
       <c r="C445" t="s">
         <v>1411</v>
       </c>
-      <c r="D445" t="s">
+      <c r="D445" s="3" t="s">
         <v>461</v>
       </c>
       <c r="E445">
@@ -26994,7 +27008,7 @@
       <c r="C446" t="s">
         <v>1411</v>
       </c>
-      <c r="D446" t="s">
+      <c r="D446" s="3" t="s">
         <v>462</v>
       </c>
       <c r="E446">
@@ -27047,7 +27061,7 @@
       <c r="C447" t="s">
         <v>1411</v>
       </c>
-      <c r="D447" t="s">
+      <c r="D447" s="3" t="s">
         <v>463</v>
       </c>
       <c r="E447">
@@ -27100,7 +27114,7 @@
       <c r="C448" t="s">
         <v>1411</v>
       </c>
-      <c r="D448" t="s">
+      <c r="D448" s="3" t="s">
         <v>464</v>
       </c>
       <c r="E448">
@@ -27153,7 +27167,7 @@
       <c r="C449" t="s">
         <v>1411</v>
       </c>
-      <c r="D449" t="s">
+      <c r="D449" s="3" t="s">
         <v>465</v>
       </c>
       <c r="E449">
@@ -27206,7 +27220,7 @@
       <c r="C450" t="s">
         <v>1411</v>
       </c>
-      <c r="D450" t="s">
+      <c r="D450" s="3" t="s">
         <v>466</v>
       </c>
       <c r="E450">
@@ -27259,7 +27273,7 @@
       <c r="C451" t="s">
         <v>1411</v>
       </c>
-      <c r="D451" t="s">
+      <c r="D451" s="2" t="s">
         <v>467</v>
       </c>
       <c r="E451">
@@ -27312,7 +27326,7 @@
       <c r="C452" t="s">
         <v>1411</v>
       </c>
-      <c r="D452" t="s">
+      <c r="D452" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E452">
@@ -27365,7 +27379,7 @@
       <c r="C453" t="s">
         <v>1411</v>
       </c>
-      <c r="D453" t="s">
+      <c r="D453" s="2" t="s">
         <v>469</v>
       </c>
       <c r="E453">
@@ -27418,7 +27432,7 @@
       <c r="C454" t="s">
         <v>1411</v>
       </c>
-      <c r="D454" t="s">
+      <c r="D454" s="2" t="s">
         <v>470</v>
       </c>
       <c r="E454">
@@ -27471,7 +27485,7 @@
       <c r="C455" t="s">
         <v>1411</v>
       </c>
-      <c r="D455" t="s">
+      <c r="D455" s="2" t="s">
         <v>471</v>
       </c>
       <c r="E455">
@@ -27524,7 +27538,7 @@
       <c r="C456" t="s">
         <v>1411</v>
       </c>
-      <c r="D456" t="s">
+      <c r="D456" s="2" t="s">
         <v>472</v>
       </c>
       <c r="E456">
@@ -27577,7 +27591,7 @@
       <c r="C457" t="s">
         <v>1411</v>
       </c>
-      <c r="D457" t="s">
+      <c r="D457" s="2" t="s">
         <v>473</v>
       </c>
       <c r="E457">
@@ -27630,7 +27644,7 @@
       <c r="C458" t="s">
         <v>1411</v>
       </c>
-      <c r="D458" t="s">
+      <c r="D458" s="2" t="s">
         <v>474</v>
       </c>
       <c r="E458">
@@ -27683,7 +27697,7 @@
       <c r="C459" t="s">
         <v>1411</v>
       </c>
-      <c r="D459" t="s">
+      <c r="D459" s="2" t="s">
         <v>475</v>
       </c>
       <c r="E459">
@@ -27736,7 +27750,7 @@
       <c r="C460" t="s">
         <v>1411</v>
       </c>
-      <c r="D460" t="s">
+      <c r="D460" s="2" t="s">
         <v>476</v>
       </c>
       <c r="E460">
@@ -27789,7 +27803,7 @@
       <c r="C461" t="s">
         <v>1411</v>
       </c>
-      <c r="D461" t="s">
+      <c r="D461" s="2" t="s">
         <v>477</v>
       </c>
       <c r="E461">
@@ -27842,7 +27856,7 @@
       <c r="C462" t="s">
         <v>1411</v>
       </c>
-      <c r="D462" t="s">
+      <c r="D462" s="2" t="s">
         <v>478</v>
       </c>
       <c r="E462">
@@ -27895,7 +27909,7 @@
       <c r="C463" t="s">
         <v>1411</v>
       </c>
-      <c r="D463" t="s">
+      <c r="D463" s="2" t="s">
         <v>479</v>
       </c>
       <c r="E463">
@@ -27948,7 +27962,7 @@
       <c r="C464" t="s">
         <v>1411</v>
       </c>
-      <c r="D464" t="s">
+      <c r="D464" s="2" t="s">
         <v>480</v>
       </c>
       <c r="E464">
@@ -28001,7 +28015,7 @@
       <c r="C465" t="s">
         <v>1411</v>
       </c>
-      <c r="D465" t="s">
+      <c r="D465" s="2" t="s">
         <v>481</v>
       </c>
       <c r="E465">
@@ -28054,7 +28068,7 @@
       <c r="C466" t="s">
         <v>1411</v>
       </c>
-      <c r="D466" t="s">
+      <c r="D466" s="2" t="s">
         <v>482</v>
       </c>
       <c r="E466">
@@ -28107,7 +28121,7 @@
       <c r="C467" t="s">
         <v>1411</v>
       </c>
-      <c r="D467" t="s">
+      <c r="D467" s="2" t="s">
         <v>483</v>
       </c>
       <c r="E467">
@@ -28160,7 +28174,7 @@
       <c r="C468" t="s">
         <v>1411</v>
       </c>
-      <c r="D468" t="s">
+      <c r="D468" s="2" t="s">
         <v>484</v>
       </c>
       <c r="E468">
@@ -28213,7 +28227,7 @@
       <c r="C469" t="s">
         <v>1411</v>
       </c>
-      <c r="D469" t="s">
+      <c r="D469" s="2" t="s">
         <v>485</v>
       </c>
       <c r="E469">
@@ -28266,7 +28280,7 @@
       <c r="C470" t="s">
         <v>1411</v>
       </c>
-      <c r="D470" t="s">
+      <c r="D470" s="2" t="s">
         <v>486</v>
       </c>
       <c r="E470">
@@ -28319,7 +28333,7 @@
       <c r="C471" t="s">
         <v>1411</v>
       </c>
-      <c r="D471" t="s">
+      <c r="D471" s="2" t="s">
         <v>487</v>
       </c>
       <c r="E471">
@@ -28372,7 +28386,7 @@
       <c r="C472" t="s">
         <v>1411</v>
       </c>
-      <c r="D472" t="s">
+      <c r="D472" s="2" t="s">
         <v>488</v>
       </c>
       <c r="E472">
@@ -28425,7 +28439,7 @@
       <c r="C473" t="s">
         <v>1411</v>
       </c>
-      <c r="D473" t="s">
+      <c r="D473" s="2" t="s">
         <v>489</v>
       </c>
       <c r="E473">
@@ -28478,7 +28492,7 @@
       <c r="C474" t="s">
         <v>1411</v>
       </c>
-      <c r="D474" t="s">
+      <c r="D474" s="2" t="s">
         <v>490</v>
       </c>
       <c r="E474">
@@ -28531,7 +28545,7 @@
       <c r="C475" t="s">
         <v>1411</v>
       </c>
-      <c r="D475" t="s">
+      <c r="D475" s="2" t="s">
         <v>491</v>
       </c>
       <c r="E475">
@@ -28584,7 +28598,7 @@
       <c r="C476" t="s">
         <v>1411</v>
       </c>
-      <c r="D476" t="s">
+      <c r="D476" s="2" t="s">
         <v>492</v>
       </c>
       <c r="E476">
@@ -28637,7 +28651,7 @@
       <c r="C477" t="s">
         <v>1411</v>
       </c>
-      <c r="D477" t="s">
+      <c r="D477" s="2" t="s">
         <v>493</v>
       </c>
       <c r="E477">
@@ -28690,7 +28704,7 @@
       <c r="C478" t="s">
         <v>1411</v>
       </c>
-      <c r="D478" t="s">
+      <c r="D478" s="2" t="s">
         <v>494</v>
       </c>
       <c r="E478">
@@ -28743,7 +28757,7 @@
       <c r="C479" t="s">
         <v>1411</v>
       </c>
-      <c r="D479" t="s">
+      <c r="D479" s="2" t="s">
         <v>495</v>
       </c>
       <c r="E479">
@@ -28796,7 +28810,7 @@
       <c r="C480" t="s">
         <v>1411</v>
       </c>
-      <c r="D480" t="s">
+      <c r="D480" s="2" t="s">
         <v>496</v>
       </c>
       <c r="E480">
@@ -28849,7 +28863,7 @@
       <c r="C481" t="s">
         <v>1411</v>
       </c>
-      <c r="D481" t="s">
+      <c r="D481" s="3" t="s">
         <v>497</v>
       </c>
       <c r="E481">
@@ -28902,7 +28916,7 @@
       <c r="C482" t="s">
         <v>1411</v>
       </c>
-      <c r="D482" t="s">
+      <c r="D482" s="3" t="s">
         <v>498</v>
       </c>
       <c r="E482">
@@ -28955,7 +28969,7 @@
       <c r="C483" t="s">
         <v>1411</v>
       </c>
-      <c r="D483" t="s">
+      <c r="D483" s="3" t="s">
         <v>499</v>
       </c>
       <c r="E483">
@@ -29008,7 +29022,7 @@
       <c r="C484" t="s">
         <v>1411</v>
       </c>
-      <c r="D484" t="s">
+      <c r="D484" s="3" t="s">
         <v>500</v>
       </c>
       <c r="E484">
@@ -29061,7 +29075,7 @@
       <c r="C485" t="s">
         <v>1411</v>
       </c>
-      <c r="D485" t="s">
+      <c r="D485" s="3" t="s">
         <v>501</v>
       </c>
       <c r="E485">
@@ -29114,7 +29128,7 @@
       <c r="C486" t="s">
         <v>1411</v>
       </c>
-      <c r="D486" t="s">
+      <c r="D486" s="3" t="s">
         <v>502</v>
       </c>
       <c r="E486">
@@ -29167,7 +29181,7 @@
       <c r="C487" t="s">
         <v>1411</v>
       </c>
-      <c r="D487" t="s">
+      <c r="D487" s="3" t="s">
         <v>503</v>
       </c>
       <c r="E487">
@@ -29220,7 +29234,7 @@
       <c r="C488" t="s">
         <v>1411</v>
       </c>
-      <c r="D488" t="s">
+      <c r="D488" s="3" t="s">
         <v>504</v>
       </c>
       <c r="E488">
@@ -29273,7 +29287,7 @@
       <c r="C489" t="s">
         <v>1411</v>
       </c>
-      <c r="D489" t="s">
+      <c r="D489" s="3" t="s">
         <v>505</v>
       </c>
       <c r="E489">
@@ -29326,7 +29340,7 @@
       <c r="C490" t="s">
         <v>1411</v>
       </c>
-      <c r="D490" t="s">
+      <c r="D490" s="3" t="s">
         <v>506</v>
       </c>
       <c r="E490">

</xml_diff>

<commit_message>
Updated on 10-30-2024 at 00:23
</commit_message>
<xml_diff>
--- a/experiment_2/data/br.xlsx
+++ b/experiment_2/data/br.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/research/LOVO/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2FA1BD-B496-864A-A386-ED8DF7DF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904607C6-9C4D-7846-B604-6E2B5C82D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4284,7 +4284,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4307,6 +4307,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE0FFE0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -4337,7 +4355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4345,6 +4363,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4611,8 +4632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P86" sqref="P86:P224"/>
+    <sheetView tabSelected="1" topLeftCell="D163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P185" sqref="P185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8374,7 +8395,7 @@
       <c r="O91">
         <v>0.107</v>
       </c>
-      <c r="P91" s="2">
+      <c r="P91" s="7">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="Q91">
@@ -8427,7 +8448,7 @@
       <c r="O92">
         <v>0.19500000000000001</v>
       </c>
-      <c r="P92" s="2">
+      <c r="P92" s="7">
         <v>0.10299999999999999</v>
       </c>
       <c r="Q92">
@@ -8480,7 +8501,7 @@
       <c r="O93">
         <v>0.186</v>
       </c>
-      <c r="P93" s="2">
+      <c r="P93" s="7">
         <v>0.122</v>
       </c>
       <c r="Q93">
@@ -8533,7 +8554,7 @@
       <c r="O94">
         <v>0.26900000000000002</v>
       </c>
-      <c r="P94" s="2">
+      <c r="P94" s="7">
         <v>0.14699999999999999</v>
       </c>
       <c r="Q94">
@@ -8586,7 +8607,7 @@
       <c r="O95">
         <v>0.27900000000000003</v>
       </c>
-      <c r="P95" s="2">
+      <c r="P95" s="7">
         <v>0.17699999999999999</v>
       </c>
       <c r="Q95">
@@ -8639,7 +8660,7 @@
       <c r="O96">
         <v>0.33900000000000002</v>
       </c>
-      <c r="P96" s="2">
+      <c r="P96" s="7">
         <v>0.21099999999999999</v>
       </c>
       <c r="Q96">
@@ -8692,7 +8713,7 @@
       <c r="O97">
         <v>0.251</v>
       </c>
-      <c r="P97" s="2">
+      <c r="P97" s="7">
         <v>0.23200000000000001</v>
       </c>
       <c r="Q97">
@@ -8745,7 +8766,7 @@
       <c r="O98">
         <v>0.311</v>
       </c>
-      <c r="P98" s="2">
+      <c r="P98" s="7">
         <v>0.26100000000000001</v>
       </c>
       <c r="Q98">
@@ -8798,7 +8819,7 @@
       <c r="O99">
         <v>0.52900000000000003</v>
       </c>
-      <c r="P99" s="2">
+      <c r="P99" s="7">
         <v>0.309</v>
       </c>
       <c r="Q99">
@@ -8851,7 +8872,7 @@
       <c r="O100">
         <v>0.61799999999999999</v>
       </c>
-      <c r="P100" s="2">
+      <c r="P100" s="7">
         <v>0.371</v>
       </c>
       <c r="Q100">
@@ -8904,7 +8925,7 @@
       <c r="O101">
         <v>0.65500000000000003</v>
       </c>
-      <c r="P101" s="2">
+      <c r="P101" s="7">
         <v>0.42599999999999999</v>
       </c>
       <c r="Q101">
@@ -8957,7 +8978,7 @@
       <c r="O102">
         <v>0.53400000000000003</v>
       </c>
-      <c r="P102" s="2">
+      <c r="P102" s="7">
         <v>0.46200000000000002</v>
       </c>
       <c r="Q102">
@@ -9010,7 +9031,7 @@
       <c r="O103">
         <v>0.316</v>
       </c>
-      <c r="P103" s="2">
+      <c r="P103" s="7">
         <v>0.45900000000000002</v>
       </c>
       <c r="Q103">
@@ -9063,7 +9084,7 @@
       <c r="O104">
         <v>0.46</v>
       </c>
-      <c r="P104" s="2">
+      <c r="P104" s="7">
         <v>0.48899999999999999</v>
       </c>
       <c r="Q104">
@@ -9116,7 +9137,7 @@
       <c r="O105">
         <v>0.48799999999999999</v>
       </c>
-      <c r="P105" s="2">
+      <c r="P105" s="7">
         <v>0.51400000000000001</v>
       </c>
       <c r="Q105">
@@ -9169,7 +9190,7 @@
       <c r="O106">
         <v>0.94699999999999995</v>
       </c>
-      <c r="P106" s="2">
+      <c r="P106" s="7">
         <v>0.57399999999999995</v>
       </c>
       <c r="Q106">
@@ -9222,7 +9243,7 @@
       <c r="O107">
         <v>0.94699999999999995</v>
       </c>
-      <c r="P107" s="2">
+      <c r="P107" s="7">
         <v>0.621</v>
       </c>
       <c r="Q107">
@@ -9275,7 +9296,7 @@
       <c r="O108">
         <v>0.873</v>
       </c>
-      <c r="P108" s="2">
+      <c r="P108" s="7">
         <v>0.65200000000000002</v>
       </c>
       <c r="Q108">
@@ -9328,7 +9349,7 @@
       <c r="O109">
         <v>1.008</v>
       </c>
-      <c r="P109" s="2">
+      <c r="P109" s="7">
         <v>0.72</v>
       </c>
       <c r="Q109">
@@ -9381,7 +9402,7 @@
       <c r="O110">
         <v>0.95699999999999996</v>
       </c>
-      <c r="P110" s="2">
+      <c r="P110" s="7">
         <v>0.81100000000000005</v>
       </c>
       <c r="Q110">
@@ -9434,7 +9455,7 @@
       <c r="O111">
         <v>0.53400000000000003</v>
       </c>
-      <c r="P111" s="2">
+      <c r="P111" s="5">
         <v>0.82199999999999995</v>
       </c>
       <c r="Q111">
@@ -9487,7 +9508,7 @@
       <c r="O112">
         <v>0.52500000000000002</v>
       </c>
-      <c r="P112" s="2">
+      <c r="P112" s="5">
         <v>0.82699999999999996</v>
       </c>
       <c r="Q112">
@@ -9540,7 +9561,7 @@
       <c r="O113">
         <v>0.77100000000000002</v>
       </c>
-      <c r="P113" s="2">
+      <c r="P113" s="5">
         <v>0.80200000000000005</v>
       </c>
       <c r="Q113">
@@ -9593,7 +9614,7 @@
       <c r="O114">
         <v>0.76600000000000001</v>
       </c>
-      <c r="P114" s="2">
+      <c r="P114" s="5">
         <v>0.77600000000000002</v>
       </c>
       <c r="Q114">
@@ -9646,7 +9667,7 @@
       <c r="O115">
         <v>1.89</v>
       </c>
-      <c r="P115" s="2">
+      <c r="P115" s="5">
         <v>0.92200000000000004</v>
       </c>
       <c r="Q115">
@@ -9699,7 +9720,7 @@
       <c r="O116">
         <v>1.6579999999999999</v>
       </c>
-      <c r="P116" s="2">
+      <c r="P116" s="5">
         <v>1.014</v>
       </c>
       <c r="Q116">
@@ -9752,7 +9773,7 @@
       <c r="O117">
         <v>1.607</v>
       </c>
-      <c r="P117" s="2">
+      <c r="P117" s="5">
         <v>1.107</v>
       </c>
       <c r="Q117">
@@ -9805,7 +9826,7 @@
       <c r="O118">
         <v>0.878</v>
       </c>
-      <c r="P118" s="2">
+      <c r="P118" s="5">
         <v>1.1559999999999999</v>
       </c>
       <c r="Q118">
@@ -9858,7 +9879,7 @@
       <c r="O119">
         <v>1.57</v>
       </c>
-      <c r="P119" s="2">
+      <c r="P119" s="5">
         <v>1.306</v>
       </c>
       <c r="Q119">
@@ -9911,7 +9932,7 @@
       <c r="O120">
         <v>2.2010000000000001</v>
       </c>
-      <c r="P120" s="2">
+      <c r="P120" s="5">
         <v>1.51</v>
       </c>
       <c r="Q120">
@@ -9964,7 +9985,7 @@
       <c r="O121">
         <v>2.085</v>
       </c>
-      <c r="P121" s="3">
+      <c r="P121" s="6">
         <v>1.6990000000000001</v>
       </c>
       <c r="Q121">
@@ -10017,7 +10038,7 @@
       <c r="O122">
         <v>2.02</v>
       </c>
-      <c r="P122" s="3">
+      <c r="P122" s="6">
         <v>1.7170000000000001</v>
       </c>
       <c r="Q122">
@@ -10070,7 +10091,7 @@
       <c r="O123">
         <v>1.988</v>
       </c>
-      <c r="P123" s="3">
+      <c r="P123" s="6">
         <v>1.764</v>
       </c>
       <c r="Q123">
@@ -10123,7 +10144,7 @@
       <c r="O124">
         <v>1.9550000000000001</v>
       </c>
-      <c r="P124" s="3">
+      <c r="P124" s="6">
         <v>1.8140000000000001</v>
       </c>
       <c r="Q124">
@@ -10176,7 +10197,7 @@
       <c r="O125">
         <v>1.2769999999999999</v>
       </c>
-      <c r="P125" s="3">
+      <c r="P125" s="6">
         <v>1.871</v>
       </c>
       <c r="Q125">
@@ -10229,7 +10250,7 @@
       <c r="O126">
         <v>1.375</v>
       </c>
-      <c r="P126" s="3">
+      <c r="P126" s="6">
         <v>1.843</v>
       </c>
       <c r="Q126">
@@ -10282,7 +10303,7 @@
       <c r="O127">
         <v>2.7869999999999999</v>
       </c>
-      <c r="P127" s="3">
+      <c r="P127" s="6">
         <v>1.927</v>
       </c>
       <c r="Q127">
@@ -10335,7 +10356,7 @@
       <c r="O128">
         <v>2.8559999999999999</v>
       </c>
-      <c r="P128" s="3">
+      <c r="P128" s="6">
         <v>2.0369999999999999</v>
       </c>
       <c r="Q128">
@@ -10388,7 +10409,7 @@
       <c r="O129">
         <v>2.8330000000000002</v>
       </c>
-      <c r="P129" s="3">
+      <c r="P129" s="6">
         <v>2.153</v>
       </c>
       <c r="Q129">
@@ -10441,7 +10462,7 @@
       <c r="O130">
         <v>3.488</v>
       </c>
-      <c r="P130" s="3">
+      <c r="P130" s="6">
         <v>2.367</v>
       </c>
       <c r="Q130">
@@ -10494,7 +10515,7 @@
       <c r="O131">
         <v>3.39</v>
       </c>
-      <c r="P131" s="3">
+      <c r="P131" s="6">
         <v>2.5720000000000001</v>
       </c>
       <c r="Q131">
@@ -10547,7 +10568,7 @@
       <c r="O132">
         <v>2.3039999999999998</v>
       </c>
-      <c r="P132" s="3">
+      <c r="P132" s="6">
         <v>2.7189999999999999</v>
       </c>
       <c r="Q132">
@@ -10600,7 +10621,7 @@
       <c r="O133">
         <v>1.839</v>
       </c>
-      <c r="P133" s="3">
+      <c r="P133" s="6">
         <v>2.7850000000000001</v>
       </c>
       <c r="Q133">
@@ -10653,7 +10674,7 @@
       <c r="O134">
         <v>4.0919999999999996</v>
       </c>
-      <c r="P134" s="3">
+      <c r="P134" s="6">
         <v>2.972</v>
       </c>
       <c r="Q134">
@@ -10706,7 +10727,7 @@
       <c r="O135">
         <v>3.4790000000000001</v>
       </c>
-      <c r="P135" s="3">
+      <c r="P135" s="6">
         <v>3.0609999999999999</v>
       </c>
       <c r="Q135">
@@ -10759,7 +10780,7 @@
       <c r="O136">
         <v>3.92</v>
       </c>
-      <c r="P136" s="3">
+      <c r="P136" s="6">
         <v>3.2160000000000002</v>
       </c>
       <c r="Q136">
@@ -10812,7 +10833,7 @@
       <c r="O137">
         <v>3.827</v>
       </c>
-      <c r="P137" s="3">
+      <c r="P137" s="6">
         <v>3.2639999999999998</v>
       </c>
       <c r="Q137">
@@ -10865,7 +10886,7 @@
       <c r="O138">
         <v>3.79</v>
       </c>
-      <c r="P138" s="3">
+      <c r="P138" s="6">
         <v>3.3210000000000002</v>
       </c>
       <c r="Q138">
@@ -10918,7 +10939,7 @@
       <c r="O139">
         <v>2.2530000000000001</v>
       </c>
-      <c r="P139" s="3">
+      <c r="P139" s="6">
         <v>3.3140000000000001</v>
       </c>
       <c r="Q139">
@@ -10971,7 +10992,7 @@
       <c r="O140">
         <v>3.13</v>
       </c>
-      <c r="P140" s="3">
+      <c r="P140" s="6">
         <v>3.4990000000000001</v>
       </c>
       <c r="Q140">
@@ -11024,7 +11045,7 @@
       <c r="O141">
         <v>5.476</v>
       </c>
-      <c r="P141" s="3">
+      <c r="P141" s="6">
         <v>3.6960000000000002</v>
       </c>
       <c r="Q141">
@@ -11077,7 +11098,7 @@
       <c r="O142">
         <v>4.1239999999999997</v>
       </c>
-      <c r="P142" s="3">
+      <c r="P142" s="6">
         <v>3.7879999999999998</v>
       </c>
       <c r="Q142">
@@ -11130,7 +11151,7 @@
       <c r="O143">
         <v>5.5179999999999998</v>
       </c>
-      <c r="P143" s="3">
+      <c r="P143" s="6">
         <v>4.0170000000000003</v>
       </c>
       <c r="Q143">
@@ -11183,7 +11204,7 @@
       <c r="O144">
         <v>4.649</v>
       </c>
-      <c r="P144" s="3">
+      <c r="P144" s="6">
         <v>4.1340000000000003</v>
       </c>
       <c r="Q144">
@@ -11236,7 +11257,7 @@
       <c r="O145">
         <v>4.4820000000000002</v>
       </c>
-      <c r="P145" s="3">
+      <c r="P145" s="6">
         <v>4.2329999999999997</v>
       </c>
       <c r="Q145">
@@ -11289,7 +11310,7 @@
       <c r="O146">
         <v>3.0329999999999999</v>
       </c>
-      <c r="P146" s="3">
+      <c r="P146" s="6">
         <v>4.3440000000000003</v>
       </c>
       <c r="Q146">
@@ -11342,7 +11363,7 @@
       <c r="O147">
         <v>3.7480000000000002</v>
       </c>
-      <c r="P147" s="3">
+      <c r="P147" s="6">
         <v>4.4329999999999998</v>
       </c>
       <c r="Q147">
@@ -11395,7 +11416,7 @@
       <c r="O148">
         <v>4.8259999999999996</v>
       </c>
-      <c r="P148" s="3">
+      <c r="P148" s="6">
         <v>4.34</v>
       </c>
       <c r="Q148">
@@ -11448,7 +11469,7 @@
       <c r="O149">
         <v>5.0439999999999996</v>
       </c>
-      <c r="P149" s="3">
+      <c r="P149" s="6">
         <v>4.4710000000000001</v>
       </c>
       <c r="Q149">
@@ -11501,7 +11522,7 @@
       <c r="O150">
         <v>5.3689999999999998</v>
       </c>
-      <c r="P150" s="3">
+      <c r="P150" s="6">
         <v>4.45</v>
       </c>
       <c r="Q150">
@@ -11554,7 +11575,7 @@
       <c r="O151">
         <v>5.22</v>
       </c>
-      <c r="P151" s="3">
+      <c r="P151" s="6">
         <v>4.532</v>
       </c>
       <c r="Q151">
@@ -11607,7 +11628,7 @@
       <c r="O152">
         <v>4.4400000000000004</v>
       </c>
-      <c r="P152" s="3">
+      <c r="P152" s="6">
         <v>4.5259999999999998</v>
       </c>
       <c r="Q152">
@@ -11660,7 +11681,7 @@
       <c r="O153">
         <v>2.2290000000000001</v>
       </c>
-      <c r="P153" s="3">
+      <c r="P153" s="6">
         <v>4.4109999999999996</v>
       </c>
       <c r="Q153">
@@ -11713,7 +11734,7 @@
       <c r="O154">
         <v>2.8929999999999998</v>
       </c>
-      <c r="P154" s="3">
+      <c r="P154" s="6">
         <v>4.2889999999999997</v>
       </c>
       <c r="Q154">
@@ -11766,7 +11787,7 @@
       <c r="O155">
         <v>5.8609999999999998</v>
       </c>
-      <c r="P155" s="3">
+      <c r="P155" s="6">
         <v>4.4370000000000003</v>
       </c>
       <c r="Q155">
@@ -11819,7 +11840,7 @@
       <c r="O156">
         <v>6.2649999999999997</v>
       </c>
-      <c r="P156" s="3">
+      <c r="P156" s="6">
         <v>4.6109999999999998</v>
       </c>
       <c r="Q156">
@@ -11872,7 +11893,7 @@
       <c r="O157">
         <v>6.8410000000000002</v>
       </c>
-      <c r="P157" s="3">
+      <c r="P157" s="6">
         <v>4.8220000000000001</v>
       </c>
       <c r="Q157">
@@ -11925,7 +11946,7 @@
       <c r="O158">
         <v>4.6680000000000001</v>
       </c>
-      <c r="P158" s="3">
+      <c r="P158" s="6">
         <v>4.7430000000000003</v>
       </c>
       <c r="Q158">
@@ -11978,7 +11999,7 @@
       <c r="O159">
         <v>4.1989999999999998</v>
       </c>
-      <c r="P159" s="3">
+      <c r="P159" s="6">
         <v>4.7080000000000002</v>
       </c>
       <c r="Q159">
@@ -12031,7 +12052,7 @@
       <c r="O160">
         <v>2.4380000000000002</v>
       </c>
-      <c r="P160" s="3">
+      <c r="P160" s="6">
         <v>4.7380000000000004</v>
       </c>
       <c r="Q160">
@@ -12084,7 +12105,7 @@
       <c r="O161">
         <v>3.1539999999999999</v>
       </c>
-      <c r="P161" s="3">
+      <c r="P161" s="6">
         <v>4.7750000000000004</v>
       </c>
       <c r="Q161">
@@ -12137,7 +12158,7 @@
       <c r="O162">
         <v>5.9080000000000004</v>
       </c>
-      <c r="P162" s="3">
+      <c r="P162" s="6">
         <v>4.782</v>
       </c>
       <c r="Q162">
@@ -12190,7 +12211,7 @@
       <c r="O163">
         <v>5.9169999999999998</v>
       </c>
-      <c r="P163" s="3">
+      <c r="P163" s="6">
         <v>4.7320000000000002</v>
       </c>
       <c r="Q163">
@@ -12243,7 +12264,7 @@
       <c r="O164">
         <v>5.7539999999999996</v>
       </c>
-      <c r="P164" s="3">
+      <c r="P164" s="6">
         <v>4.577</v>
       </c>
       <c r="Q164">
@@ -12296,7 +12317,7 @@
       <c r="O165">
         <v>4.2220000000000004</v>
       </c>
-      <c r="P165" s="3">
+      <c r="P165" s="6">
         <v>4.5129999999999999</v>
       </c>
       <c r="Q165">
@@ -12349,7 +12370,7 @@
       <c r="O166">
         <v>4.1429999999999998</v>
       </c>
-      <c r="P166" s="3">
+      <c r="P166" s="6">
         <v>4.5049999999999999</v>
       </c>
       <c r="Q166">
@@ -12402,7 +12423,7 @@
       <c r="O167">
         <v>2.8420000000000001</v>
       </c>
-      <c r="P167" s="3">
+      <c r="P167" s="6">
         <v>4.5629999999999997</v>
       </c>
       <c r="Q167">
@@ -12455,7 +12476,7 @@
       <c r="O168">
         <v>2.9119999999999999</v>
       </c>
-      <c r="P168" s="3">
+      <c r="P168" s="6">
         <v>4.5279999999999996</v>
       </c>
       <c r="Q168">
@@ -12508,7 +12529,7 @@
       <c r="O169">
         <v>5.9539999999999997</v>
       </c>
-      <c r="P169" s="3">
+      <c r="P169" s="6">
         <v>4.5350000000000001</v>
       </c>
       <c r="Q169">
@@ -12561,7 +12582,7 @@
       <c r="O170">
         <v>5.8940000000000001</v>
       </c>
-      <c r="P170" s="3">
+      <c r="P170" s="6">
         <v>4.532</v>
       </c>
       <c r="Q170">
@@ -12614,7 +12635,7 @@
       <c r="O171">
         <v>5.75</v>
       </c>
-      <c r="P171" s="3">
+      <c r="P171" s="6">
         <v>4.5309999999999997</v>
       </c>
       <c r="Q171">
@@ -12667,7 +12688,7 @@
       <c r="O172">
         <v>5.601</v>
       </c>
-      <c r="P172" s="3">
+      <c r="P172" s="6">
         <v>4.7279999999999998</v>
       </c>
       <c r="Q172">
@@ -12720,7 +12741,7 @@
       <c r="O173">
         <v>4.7469999999999999</v>
       </c>
-      <c r="P173" s="3">
+      <c r="P173" s="6">
         <v>4.8140000000000001</v>
       </c>
       <c r="Q173">
@@ -12773,7 +12794,7 @@
       <c r="O174">
         <v>2.9769999999999999</v>
       </c>
-      <c r="P174" s="3">
+      <c r="P174" s="6">
         <v>4.8330000000000002</v>
       </c>
       <c r="Q174">
@@ -12826,7 +12847,7 @@
       <c r="O175">
         <v>3.0369999999999999</v>
       </c>
-      <c r="P175" s="3">
+      <c r="P175" s="6">
         <v>4.851</v>
       </c>
       <c r="Q175">
@@ -12879,7 +12900,7 @@
       <c r="O176">
         <v>6.3810000000000002</v>
       </c>
-      <c r="P176" s="3">
+      <c r="P176" s="6">
         <v>4.9119999999999999</v>
       </c>
       <c r="Q176">
@@ -12932,7 +12953,7 @@
       <c r="O177">
         <v>5.5039999999999996</v>
       </c>
-      <c r="P177" s="3">
+      <c r="P177" s="6">
         <v>4.8570000000000002</v>
       </c>
       <c r="Q177">
@@ -12985,7 +13006,7 @@
       <c r="O178">
         <v>5.2990000000000004</v>
       </c>
-      <c r="P178" s="3">
+      <c r="P178" s="6">
         <v>4.7919999999999998</v>
       </c>
       <c r="Q178">
@@ -13038,7 +13059,7 @@
       <c r="O179">
         <v>4.5979999999999999</v>
       </c>
-      <c r="P179" s="3">
+      <c r="P179" s="6">
         <v>4.649</v>
       </c>
       <c r="Q179">
@@ -13091,7 +13112,7 @@
       <c r="O180">
         <v>5.1509999999999998</v>
       </c>
-      <c r="P180" s="3">
+      <c r="P180" s="6">
         <v>4.7069999999999999</v>
       </c>
       <c r="Q180">
@@ -13144,7 +13165,7 @@
       <c r="O181">
         <v>2.5640000000000001</v>
       </c>
-      <c r="P181" s="3">
+      <c r="P181" s="6">
         <v>4.6479999999999997</v>
       </c>
       <c r="Q181">
@@ -13197,7 +13218,7 @@
       <c r="O182">
         <v>3.214</v>
       </c>
-      <c r="P182" s="3">
+      <c r="P182" s="6">
         <v>4.673</v>
       </c>
       <c r="Q182">
@@ -13250,7 +13271,7 @@
       <c r="O183">
         <v>5.9450000000000003</v>
       </c>
-      <c r="P183" s="3">
+      <c r="P183" s="6">
         <v>4.6109999999999998</v>
       </c>
       <c r="Q183">
@@ -13303,7 +13324,7 @@
       <c r="O184">
         <v>4.8209999999999997</v>
       </c>
-      <c r="P184" s="3">
+      <c r="P184" s="6">
         <v>4.5129999999999999</v>
       </c>
       <c r="Q184">
@@ -13356,7 +13377,7 @@
       <c r="O185">
         <v>5.8150000000000004</v>
       </c>
-      <c r="P185" s="3">
+      <c r="P185" s="6">
         <v>4.5869999999999997</v>
       </c>
       <c r="Q185">

</xml_diff>

<commit_message>
Updated on 11-03-2024 at 22:53
</commit_message>
<xml_diff>
--- a/experiment_2/data/br.xlsx
+++ b/experiment_2/data/br.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/research/LOVO/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32EBB6C-0557-5E4A-9537-E9793F73F897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC5CBC7-ED0F-2E4E-9821-D3569CB02897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-4260" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4667,8 +4667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q213" sqref="Q213"/>
+    <sheetView tabSelected="1" topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R107" sqref="R107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14475,7 +14475,7 @@
       <c r="O205" s="8">
         <v>5.9630000000000001</v>
       </c>
-      <c r="P205" s="5">
+      <c r="P205" s="11">
         <v>4.9130000000000003</v>
       </c>
       <c r="Q205">
@@ -14528,7 +14528,7 @@
       <c r="O206" s="8">
         <v>6.0890000000000004</v>
       </c>
-      <c r="P206" s="5">
+      <c r="P206" s="11">
         <v>4.9059999999999997</v>
       </c>
       <c r="Q206">
@@ -14581,7 +14581,7 @@
       <c r="O207" s="8">
         <v>5.3689999999999998</v>
       </c>
-      <c r="P207" s="5">
+      <c r="P207" s="11">
         <v>4.9009999999999998</v>
       </c>
       <c r="Q207">
@@ -14634,7 +14634,7 @@
       <c r="O208" s="8">
         <v>5.6239999999999997</v>
       </c>
-      <c r="P208" s="5">
+      <c r="P208" s="11">
         <v>5.0940000000000003</v>
       </c>
       <c r="Q208">

</xml_diff>

<commit_message>
Updated on 12-09-2024 at 09:14
</commit_message>
<xml_diff>
--- a/experiment_2/data/br.xlsx
+++ b/experiment_2/data/br.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/research/LOVO/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17C51BF-E41E-C845-BCD7-F92528682A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D6A5D5-E32C-B64A-B488-FE4324F846C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="-18740" windowWidth="21600" windowHeight="37900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4688,8 +4688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D174" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V191" sqref="V191"/>
+    <sheetView tabSelected="1" topLeftCell="D110" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P169" sqref="P165:P169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>